<commit_message>
se corrige columna name de Staff
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7267EF1E-E5DA-1C44-8915-2C47373D69AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74941AC1-BAE5-B141-8AF7-989E95D70D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="25800" windowHeight="26720" activeTab="2" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
+    <workbookView xWindow="21100" yWindow="500" windowWidth="25800" windowHeight="26720" activeTab="2" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="430">
   <si>
     <t>Modalidad</t>
   </si>
@@ -923,6 +923,423 @@
   </si>
   <si>
     <t>DocumentID</t>
+  </si>
+  <si>
+    <t>Adriana Casas Caro</t>
+  </si>
+  <si>
+    <t>Adriana Marcela Villamarín Rodríguez</t>
+  </si>
+  <si>
+    <t>Adriana María Páez Gallego</t>
+  </si>
+  <si>
+    <t>Adriana Silveira Jaramillo</t>
+  </si>
+  <si>
+    <t>Aida María Castañeda Parra</t>
+  </si>
+  <si>
+    <t>Alfredo Pachón Soler</t>
+  </si>
+  <si>
+    <t>Álvaro Ernesto Rivera Bustos</t>
+  </si>
+  <si>
+    <t>Ana María Cárdenas Montenegro</t>
+  </si>
+  <si>
+    <t>Ana María Iturralde Sánchez</t>
+  </si>
+  <si>
+    <t>Ana María Pérez Díaz</t>
+  </si>
+  <si>
+    <t>Ana Mylena Gómez Arango</t>
+  </si>
+  <si>
+    <t>Anderson Mantilla Vasquez</t>
+  </si>
+  <si>
+    <t>Andrés Arturo Torres Amado</t>
+  </si>
+  <si>
+    <t>Andrés Felipe Guerrero Quintero</t>
+  </si>
+  <si>
+    <t>Andrés Huertas Motta</t>
+  </si>
+  <si>
+    <t>Anna Zakorchemney</t>
+  </si>
+  <si>
+    <t>Beatrice Nenuca Adarme Gevarra</t>
+  </si>
+  <si>
+    <t>Berlly Nallive Ospina Vasco</t>
+  </si>
+  <si>
+    <t>Blanca Inés Cañón Nieto</t>
+  </si>
+  <si>
+    <t>Camila Arango Ordóñez</t>
+  </si>
+  <si>
+    <t>Camila Fuentes Díaz</t>
+  </si>
+  <si>
+    <t>Camilo Ernesto Joya Benítez</t>
+  </si>
+  <si>
+    <t>Camilo Herrera Téllez</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo Blanco López</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo Carvajal Nieto</t>
+  </si>
+  <si>
+    <t>Carmen Diana Leslye Raymond Ángel</t>
+  </si>
+  <si>
+    <t>Catalina Rodríguez Parra</t>
+  </si>
+  <si>
+    <t>Claudia Gaitán McAllister</t>
+  </si>
+  <si>
+    <t>Claudia Milena Buitrago Peña</t>
+  </si>
+  <si>
+    <t>Claudia Pilar Grass Hoyos</t>
+  </si>
+  <si>
+    <t>Daniel Alberto Vergel Bedoya</t>
+  </si>
+  <si>
+    <t>Daniel Cammaert Hurtado</t>
+  </si>
+  <si>
+    <t>Daniela García Chacón</t>
+  </si>
+  <si>
+    <t>Daniella Ferroni Calderón</t>
+  </si>
+  <si>
+    <t>Denisse Giraud López</t>
+  </si>
+  <si>
+    <t>Diana Lucía Salas Quijano</t>
+  </si>
+  <si>
+    <t>Doris Marcela Guayacán Rincón</t>
+  </si>
+  <si>
+    <t>Erika Giovanna Leguizamón Pachón</t>
+  </si>
+  <si>
+    <t>Erika Johana Arnáiz Caballero</t>
+  </si>
+  <si>
+    <t>Esperanza Caro Restrepo</t>
+  </si>
+  <si>
+    <t>Esperanza Comia Cardenas</t>
+  </si>
+  <si>
+    <t>Farid Ignacio Salgado Cajales</t>
+  </si>
+  <si>
+    <t>Farley del Socorro Durán Acosta</t>
+  </si>
+  <si>
+    <t>Francia Shenedy Contreras Cañón</t>
+  </si>
+  <si>
+    <t>Francy Rodríguez Saavedra</t>
+  </si>
+  <si>
+    <t>Giovanna Fragale Castillo</t>
+  </si>
+  <si>
+    <t>Gladys Natalia Quemba Rubio</t>
+  </si>
+  <si>
+    <t>Gonzalo Iván Ocampo Yepes</t>
+  </si>
+  <si>
+    <t>Hans Jacobsohn Forero</t>
+  </si>
+  <si>
+    <t>Hugo Arbey Cely Moya</t>
+  </si>
+  <si>
+    <t>Jeannette Gleiser Dobrzynski</t>
+  </si>
+  <si>
+    <t>Jenny Edith Murcia Rodríguez</t>
+  </si>
+  <si>
+    <t>Jenny Milena Herrera Jiménez</t>
+  </si>
+  <si>
+    <t>Jesús Orlando Guerrero Pabón</t>
+  </si>
+  <si>
+    <t>John Hardy Olaya Osorio</t>
+  </si>
+  <si>
+    <t>Jonathan Iván Mora Rueda</t>
+  </si>
+  <si>
+    <t>Jorge Enrique Guachetá Ramírez</t>
+  </si>
+  <si>
+    <t>José Fernando Castillo Reina</t>
+  </si>
+  <si>
+    <t>José María Armenta Crespo</t>
+  </si>
+  <si>
+    <t>Juan Nicolás Jaramillo Ramírez</t>
+  </si>
+  <si>
+    <t>Juan Nicolás Leguizamón Russi</t>
+  </si>
+  <si>
+    <t>Juan Sebastián Salamanca Zapata</t>
+  </si>
+  <si>
+    <t>Juana Amaya Villaneda</t>
+  </si>
+  <si>
+    <t>Juanita Alford Alford</t>
+  </si>
+  <si>
+    <t>Juliana Arias García</t>
+  </si>
+  <si>
+    <t>Juliana del Pilar Pinzón Vargas</t>
+  </si>
+  <si>
+    <t>Juliana Gordillo Gómez</t>
+  </si>
+  <si>
+    <t>Julio Enrique Cabrales Durán</t>
+  </si>
+  <si>
+    <t>Keshia Nicole Angie Castillo Visbal</t>
+  </si>
+  <si>
+    <t>Lady Diana Hernández Arévalo</t>
+  </si>
+  <si>
+    <t>Laura Angélica Pulido Ortiz</t>
+  </si>
+  <si>
+    <t>Laura Isabel Sandino Garcés</t>
+  </si>
+  <si>
+    <t>Laura Jimena Isaza Herrera</t>
+  </si>
+  <si>
+    <t>Laura Jiménez Hakim</t>
+  </si>
+  <si>
+    <t>Laura Murillo Torres</t>
+  </si>
+  <si>
+    <t>Laura Sofía Velandia Torres</t>
+  </si>
+  <si>
+    <t>Lenis Isabel Barrios Mendoza</t>
+  </si>
+  <si>
+    <t>Leonardo Cabas Manjarres</t>
+  </si>
+  <si>
+    <t>Liliana Cortés Reinel</t>
+  </si>
+  <si>
+    <t>Lucía Kristine Umbreit Caballero</t>
+  </si>
+  <si>
+    <t>Luis Alberto Sicuamia Pineda</t>
+  </si>
+  <si>
+    <t>Luisa Fernanda Calvo Pedraza</t>
+  </si>
+  <si>
+    <t>Luz Adriana Pinzón Orjuela</t>
+  </si>
+  <si>
+    <t>Luz Marina Peñaranda Torrado</t>
+  </si>
+  <si>
+    <t>Luz Patricia Daza</t>
+  </si>
+  <si>
+    <t>Luz Yenith Rodríguez Téllez</t>
+  </si>
+  <si>
+    <t>Magdalena Jiménez Hakim</t>
+  </si>
+  <si>
+    <t>Marcela Cabarcas Parra</t>
+  </si>
+  <si>
+    <t>María Angélica Álvarez Castro</t>
+  </si>
+  <si>
+    <t>María Camila Carvajal Nieto</t>
+  </si>
+  <si>
+    <t>María Consuelo Giraldo Hurtado</t>
+  </si>
+  <si>
+    <t>María del Pilar Díaz Rincón</t>
+  </si>
+  <si>
+    <t>María del Sol Peralta Vasco</t>
+  </si>
+  <si>
+    <t>María Emilia Garcés Venegas</t>
+  </si>
+  <si>
+    <t>Maria Fernanda Crespo Cordovez</t>
+  </si>
+  <si>
+    <t>María Inés Romero Caro</t>
+  </si>
+  <si>
+    <t>María Paula Sánchez Gil</t>
+  </si>
+  <si>
+    <t>Maria Paulina Jaramillo Ramírez</t>
+  </si>
+  <si>
+    <t>María Pronina</t>
+  </si>
+  <si>
+    <t>Maria Teresa Botero Medina</t>
+  </si>
+  <si>
+    <t>María Teresa García Vásquez</t>
+  </si>
+  <si>
+    <t>Mariela Josefina García Cardona</t>
+  </si>
+  <si>
+    <t>Martha Cecilia Gómez Serna</t>
+  </si>
+  <si>
+    <t>Martha Juliana Galvis Galeano</t>
+  </si>
+  <si>
+    <t>Martha Liliana García Dávila</t>
+  </si>
+  <si>
+    <t>Martha Lucía Calero Marquez</t>
+  </si>
+  <si>
+    <t>Martha Lucía Obando Moreno</t>
+  </si>
+  <si>
+    <t>Mayra Alejandra Bermúdez Martín</t>
+  </si>
+  <si>
+    <t>Mireya Adriana Londoño Correal</t>
+  </si>
+  <si>
+    <t>Nathaly Font Prieto</t>
+  </si>
+  <si>
+    <t>Nelson Yamid Molano Pinzón</t>
+  </si>
+  <si>
+    <t>Néstor Orlando León Santibáñez</t>
+  </si>
+  <si>
+    <t>Nidia Margoth Guevara Rojas</t>
+  </si>
+  <si>
+    <t>Olga Lucia Campos Naranjo</t>
+  </si>
+  <si>
+    <t>Omar John Fuquen Fonseca</t>
+  </si>
+  <si>
+    <t>Oscar Eduardo Jaimes Gómez</t>
+  </si>
+  <si>
+    <t>Paul Kelly</t>
+  </si>
+  <si>
+    <t>Pauline Ara Obale</t>
+  </si>
+  <si>
+    <t>René Alejandro Garizzao Henao</t>
+  </si>
+  <si>
+    <t>Robert Hernán Acevedo Medina</t>
+  </si>
+  <si>
+    <t>Robin Clairese Duke</t>
+  </si>
+  <si>
+    <t>Rosa Cecilia Caro Restrepo</t>
+  </si>
+  <si>
+    <t>Sandra Liliana Salamanca Flautero</t>
+  </si>
+  <si>
+    <t>Sandra Patricia Cristiano Nieto</t>
+  </si>
+  <si>
+    <t>Sandra Patricia Ramírez Vargas</t>
+  </si>
+  <si>
+    <t>Sara Elena Torres Mogollón</t>
+  </si>
+  <si>
+    <t>Silvia Dever Fonnegra</t>
+  </si>
+  <si>
+    <t>Simón Ganitsky White</t>
+  </si>
+  <si>
+    <t>Sol Nancy Cardozo Muñoz</t>
+  </si>
+  <si>
+    <t>Sonia Esperanza Guerrero Sánchez</t>
+  </si>
+  <si>
+    <t>Stephanie Whitefield Gravina</t>
+  </si>
+  <si>
+    <t>Verónica Nempeque Lizarazo</t>
+  </si>
+  <si>
+    <t>Wendy Alexandra Atencio Castrillo</t>
+  </si>
+  <si>
+    <t>Xiris Paola Leon Vargas</t>
+  </si>
+  <si>
+    <t>Yaneth Ordóñez Salinas</t>
+  </si>
+  <si>
+    <t>Yaneth Rocío Muñoz Campos</t>
+  </si>
+  <si>
+    <t>Yenny Catalina Daza Melo</t>
+  </si>
+  <si>
+    <t>Yina Marcela Arias Moreno</t>
+  </si>
+  <si>
+    <t>Zuly Vanessa Pérez Pinzón</t>
   </si>
 </sst>
 </file>
@@ -2148,7 +2565,7 @@
   <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2189,7 +2606,7 @@
         <v>41</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>41</v>
+        <v>291</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>41</v>
@@ -2209,7 +2626,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>123</v>
@@ -2229,7 +2646,7 @@
         <v>256</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>256</v>
@@ -2246,7 +2663,7 @@
         <v>119</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>119</v>
+        <v>294</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>119</v>
@@ -2266,7 +2683,7 @@
         <v>42</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>42</v>
@@ -2286,7 +2703,7 @@
         <v>104</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>104</v>
+        <v>296</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>104</v>
@@ -2306,7 +2723,7 @@
         <v>111</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>111</v>
+        <v>297</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>111</v>
@@ -2326,7 +2743,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>37</v>
+        <v>298</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>37</v>
@@ -2346,7 +2763,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>80</v>
+        <v>299</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>80</v>
@@ -2366,7 +2783,7 @@
         <v>257</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>257</v>
+        <v>300</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>257</v>
@@ -2386,7 +2803,7 @@
         <v>66</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>66</v>
+        <v>301</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>66</v>
@@ -2406,7 +2823,7 @@
         <v>258</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>258</v>
+        <v>302</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>258</v>
@@ -2426,7 +2843,7 @@
         <v>120</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>120</v>
+        <v>303</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>120</v>
@@ -2446,7 +2863,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>73</v>
+        <v>304</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>73</v>
@@ -2466,7 +2883,7 @@
         <v>78</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>78</v>
+        <v>305</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>78</v>
@@ -2486,7 +2903,7 @@
         <v>125</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>125</v>
+        <v>306</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>125</v>
@@ -2506,7 +2923,7 @@
         <v>259</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>259</v>
+        <v>307</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>259</v>
@@ -2526,7 +2943,7 @@
         <v>103</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>103</v>
@@ -2546,7 +2963,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>36</v>
+        <v>309</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>36</v>
@@ -2566,7 +2983,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>21</v>
@@ -2586,7 +3003,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>54</v>
@@ -2606,7 +3023,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>86</v>
+        <v>312</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>86</v>
@@ -2626,7 +3043,7 @@
         <v>77</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>77</v>
+        <v>313</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>77</v>
@@ -2646,7 +3063,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>28</v>
+        <v>314</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>28</v>
@@ -2666,7 +3083,7 @@
         <v>260</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>260</v>
+        <v>315</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>260</v>
@@ -2686,7 +3103,7 @@
         <v>110</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>110</v>
+        <v>316</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>110</v>
@@ -2706,7 +3123,7 @@
         <v>261</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>261</v>
@@ -2726,7 +3143,7 @@
         <v>56</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>56</v>
@@ -2746,7 +3163,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>30</v>
+        <v>319</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>30</v>
@@ -2766,7 +3183,7 @@
         <v>69</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="D31" s="21" t="s">
         <v>69</v>
@@ -2786,7 +3203,7 @@
         <v>122</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>122</v>
+        <v>321</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>122</v>
@@ -2806,7 +3223,7 @@
         <v>262</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>262</v>
+        <v>322</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>262</v>
@@ -2826,7 +3243,7 @@
         <v>263</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>263</v>
+        <v>323</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>263</v>
@@ -2846,7 +3263,7 @@
         <v>52</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>52</v>
+        <v>324</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>52</v>
@@ -2866,7 +3283,7 @@
         <v>64</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>64</v>
+        <v>325</v>
       </c>
       <c r="D36" s="21" t="s">
         <v>64</v>
@@ -2886,7 +3303,7 @@
         <v>115</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>115</v>
@@ -2906,7 +3323,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>71</v>
+        <v>327</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>71</v>
@@ -2926,7 +3343,7 @@
         <v>88</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>88</v>
+        <v>328</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>88</v>
@@ -2946,7 +3363,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>25</v>
@@ -2966,7 +3383,7 @@
         <v>264</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>264</v>
+        <v>330</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>264</v>
@@ -2986,7 +3403,7 @@
         <v>265</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>265</v>
+        <v>331</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>265</v>
@@ -3006,7 +3423,7 @@
         <v>116</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>116</v>
+        <v>332</v>
       </c>
       <c r="D43" s="21" t="s">
         <v>116</v>
@@ -3026,7 +3443,7 @@
         <v>51</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>51</v>
+        <v>333</v>
       </c>
       <c r="D44" s="21" t="s">
         <v>51</v>
@@ -3046,7 +3463,7 @@
         <v>266</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>266</v>
+        <v>334</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>266</v>
@@ -3066,7 +3483,7 @@
         <v>267</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>267</v>
+        <v>335</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>267</v>
@@ -3086,7 +3503,7 @@
         <v>268</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>268</v>
+        <v>336</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>268</v>
@@ -3106,7 +3523,7 @@
         <v>269</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>269</v>
+        <v>337</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>269</v>
@@ -3126,7 +3543,7 @@
         <v>100</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>100</v>
+        <v>338</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>100</v>
@@ -3146,7 +3563,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>81</v>
+        <v>339</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>81</v>
@@ -3166,7 +3583,7 @@
         <v>45</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>45</v>
+        <v>340</v>
       </c>
       <c r="D51" s="21" t="s">
         <v>45</v>
@@ -3186,7 +3603,7 @@
         <v>65</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>65</v>
+        <v>341</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>65</v>
@@ -3206,7 +3623,7 @@
         <v>96</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>96</v>
+        <v>342</v>
       </c>
       <c r="D53" s="21" t="s">
         <v>96</v>
@@ -3226,7 +3643,7 @@
         <v>270</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>270</v>
+        <v>343</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>270</v>
@@ -3246,7 +3663,7 @@
         <v>72</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>72</v>
+        <v>344</v>
       </c>
       <c r="D55" s="21" t="s">
         <v>72</v>
@@ -3266,7 +3683,7 @@
         <v>101</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>101</v>
+        <v>345</v>
       </c>
       <c r="D56" s="21" t="s">
         <v>101</v>
@@ -3286,7 +3703,7 @@
         <v>94</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>94</v>
+        <v>346</v>
       </c>
       <c r="D57" s="21" t="s">
         <v>94</v>
@@ -3306,7 +3723,7 @@
         <v>70</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>70</v>
+        <v>347</v>
       </c>
       <c r="D58" s="21" t="s">
         <v>70</v>
@@ -3326,7 +3743,7 @@
         <v>43</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>43</v>
+        <v>348</v>
       </c>
       <c r="D59" s="21" t="s">
         <v>43</v>
@@ -3346,7 +3763,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>24</v>
+        <v>349</v>
       </c>
       <c r="D60" s="21" t="s">
         <v>24</v>
@@ -3366,7 +3783,7 @@
         <v>82</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>82</v>
+        <v>350</v>
       </c>
       <c r="D61" s="21" t="s">
         <v>82</v>
@@ -3386,7 +3803,7 @@
         <v>89</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>89</v>
+        <v>351</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>89</v>
@@ -3406,7 +3823,7 @@
         <v>271</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>271</v>
+        <v>352</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>271</v>
@@ -3426,7 +3843,7 @@
         <v>272</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>272</v>
+        <v>353</v>
       </c>
       <c r="D64" s="21" t="s">
         <v>272</v>
@@ -3446,7 +3863,7 @@
         <v>273</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>273</v>
+        <v>354</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>273</v>
@@ -3466,7 +3883,7 @@
         <v>22</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>22</v>
+        <v>355</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>22</v>
@@ -3486,7 +3903,7 @@
         <v>107</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>107</v>
+        <v>356</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>107</v>
@@ -3506,7 +3923,7 @@
         <v>68</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>68</v>
+        <v>357</v>
       </c>
       <c r="D68" s="21" t="s">
         <v>68</v>
@@ -3526,7 +3943,7 @@
         <v>33</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>33</v>
+        <v>358</v>
       </c>
       <c r="D69" s="21" t="s">
         <v>33</v>
@@ -3546,7 +3963,7 @@
         <v>44</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>44</v>
+        <v>359</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>44</v>
@@ -3566,7 +3983,7 @@
         <v>76</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>76</v>
+        <v>360</v>
       </c>
       <c r="D71" s="21" t="s">
         <v>76</v>
@@ -3586,7 +4003,7 @@
         <v>108</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>108</v>
+        <v>361</v>
       </c>
       <c r="D72" s="21" t="s">
         <v>108</v>
@@ -3606,7 +4023,7 @@
         <v>274</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>274</v>
+        <v>362</v>
       </c>
       <c r="D73" s="21" t="s">
         <v>274</v>
@@ -3626,7 +4043,7 @@
         <v>79</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>79</v>
+        <v>363</v>
       </c>
       <c r="D74" s="21" t="s">
         <v>79</v>
@@ -3646,7 +4063,7 @@
         <v>84</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>84</v>
+        <v>364</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>84</v>
@@ -3666,7 +4083,7 @@
         <v>97</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>97</v>
+        <v>365</v>
       </c>
       <c r="D76" s="21" t="s">
         <v>97</v>
@@ -3686,7 +4103,7 @@
         <v>275</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>275</v>
+        <v>366</v>
       </c>
       <c r="D77" s="21" t="s">
         <v>275</v>
@@ -3706,7 +4123,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>27</v>
+        <v>367</v>
       </c>
       <c r="D78" s="21" t="s">
         <v>27</v>
@@ -3726,7 +4143,7 @@
         <v>32</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>32</v>
+        <v>368</v>
       </c>
       <c r="D79" s="21" t="s">
         <v>32</v>
@@ -3746,7 +4163,7 @@
         <v>276</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>276</v>
+        <v>369</v>
       </c>
       <c r="D80" s="21" t="s">
         <v>276</v>
@@ -3766,7 +4183,7 @@
         <v>121</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>121</v>
+        <v>370</v>
       </c>
       <c r="D81" s="21" t="s">
         <v>121</v>
@@ -3786,7 +4203,7 @@
         <v>118</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>118</v>
+        <v>371</v>
       </c>
       <c r="D82" s="22" t="s">
         <v>118</v>
@@ -3806,7 +4223,7 @@
         <v>35</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>35</v>
+        <v>372</v>
       </c>
       <c r="D83" s="21" t="s">
         <v>35</v>
@@ -3826,7 +4243,7 @@
         <v>106</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>106</v>
+        <v>373</v>
       </c>
       <c r="D84" s="21" t="s">
         <v>106</v>
@@ -3846,7 +4263,7 @@
         <v>277</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>277</v>
+        <v>374</v>
       </c>
       <c r="D85" s="21" t="s">
         <v>277</v>
@@ -3866,7 +4283,7 @@
         <v>47</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>47</v>
+        <v>375</v>
       </c>
       <c r="D86" s="21" t="s">
         <v>47</v>
@@ -3886,7 +4303,7 @@
         <v>112</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>112</v>
+        <v>376</v>
       </c>
       <c r="D87" s="21" t="s">
         <v>112</v>
@@ -3906,7 +4323,7 @@
         <v>85</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>85</v>
+        <v>377</v>
       </c>
       <c r="D88" s="21" t="s">
         <v>85</v>
@@ -3926,7 +4343,7 @@
         <v>31</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>31</v>
+        <v>378</v>
       </c>
       <c r="D89" s="21" t="s">
         <v>31</v>
@@ -3946,7 +4363,7 @@
         <v>278</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>278</v>
+        <v>379</v>
       </c>
       <c r="D90" s="21" t="s">
         <v>278</v>
@@ -3966,7 +4383,7 @@
         <v>279</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>279</v>
+        <v>380</v>
       </c>
       <c r="D91" s="21" t="s">
         <v>279</v>
@@ -3986,7 +4403,7 @@
         <v>63</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>63</v>
+        <v>381</v>
       </c>
       <c r="D92" s="21" t="s">
         <v>63</v>
@@ -4006,7 +4423,7 @@
         <v>50</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>50</v>
+        <v>382</v>
       </c>
       <c r="D93" s="21" t="s">
         <v>50</v>
@@ -4026,7 +4443,7 @@
         <v>105</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>105</v>
+        <v>383</v>
       </c>
       <c r="D94" s="22" t="s">
         <v>105</v>
@@ -4046,7 +4463,7 @@
         <v>59</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>59</v>
+        <v>384</v>
       </c>
       <c r="D95" s="21" t="s">
         <v>59</v>
@@ -4066,7 +4483,7 @@
         <v>280</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>280</v>
+        <v>385</v>
       </c>
       <c r="D96" s="21" t="s">
         <v>280</v>
@@ -4086,7 +4503,7 @@
         <v>113</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>113</v>
+        <v>386</v>
       </c>
       <c r="D97" s="21" t="s">
         <v>113</v>
@@ -4106,7 +4523,7 @@
         <v>117</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>117</v>
+        <v>387</v>
       </c>
       <c r="D98" s="21" t="s">
         <v>117</v>
@@ -4126,7 +4543,7 @@
         <v>83</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>83</v>
+        <v>388</v>
       </c>
       <c r="D99" s="21" t="s">
         <v>83</v>
@@ -4146,7 +4563,7 @@
         <v>281</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>281</v>
+        <v>389</v>
       </c>
       <c r="D100" s="21" t="s">
         <v>281</v>
@@ -4166,7 +4583,7 @@
         <v>29</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>29</v>
+        <v>390</v>
       </c>
       <c r="D101" s="21" t="s">
         <v>29</v>
@@ -4186,7 +4603,7 @@
         <v>61</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>61</v>
+        <v>391</v>
       </c>
       <c r="D102" s="21" t="s">
         <v>61</v>
@@ -4206,7 +4623,7 @@
         <v>60</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>60</v>
+        <v>392</v>
       </c>
       <c r="D103" s="21" t="s">
         <v>60</v>
@@ -4226,7 +4643,7 @@
         <v>67</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>67</v>
+        <v>393</v>
       </c>
       <c r="D104" s="21" t="s">
         <v>67</v>
@@ -4246,7 +4663,7 @@
         <v>57</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>57</v>
+        <v>394</v>
       </c>
       <c r="D105" s="21" t="s">
         <v>57</v>
@@ -4266,7 +4683,7 @@
         <v>282</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>282</v>
+        <v>395</v>
       </c>
       <c r="D106" s="21" t="s">
         <v>282</v>
@@ -4286,7 +4703,7 @@
         <v>34</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>34</v>
+        <v>396</v>
       </c>
       <c r="D107" s="21" t="s">
         <v>34</v>
@@ -4306,7 +4723,7 @@
         <v>99</v>
       </c>
       <c r="C108" s="21" t="s">
-        <v>99</v>
+        <v>397</v>
       </c>
       <c r="D108" s="21" t="s">
         <v>99</v>
@@ -4326,7 +4743,7 @@
         <v>283</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>283</v>
+        <v>398</v>
       </c>
       <c r="D109" s="21" t="s">
         <v>283</v>
@@ -4346,7 +4763,7 @@
         <v>92</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>92</v>
+        <v>399</v>
       </c>
       <c r="D110" s="21" t="s">
         <v>92</v>
@@ -4366,7 +4783,7 @@
         <v>53</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>53</v>
+        <v>400</v>
       </c>
       <c r="D111" s="21" t="s">
         <v>53</v>
@@ -4386,7 +4803,7 @@
         <v>93</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>93</v>
+        <v>401</v>
       </c>
       <c r="D112" s="21" t="s">
         <v>93</v>
@@ -4406,7 +4823,7 @@
         <v>90</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>90</v>
+        <v>402</v>
       </c>
       <c r="D113" s="21" t="s">
         <v>90</v>
@@ -4426,7 +4843,7 @@
         <v>75</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>75</v>
+        <v>403</v>
       </c>
       <c r="D114" s="21" t="s">
         <v>75</v>
@@ -4446,7 +4863,7 @@
         <v>284</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>284</v>
+        <v>404</v>
       </c>
       <c r="D115" s="21" t="s">
         <v>284</v>
@@ -4466,7 +4883,7 @@
         <v>55</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>55</v>
+        <v>405</v>
       </c>
       <c r="D116" s="21" t="s">
         <v>55</v>
@@ -4486,7 +4903,7 @@
         <v>285</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>285</v>
+        <v>406</v>
       </c>
       <c r="D117" s="21" t="s">
         <v>285</v>
@@ -4506,7 +4923,7 @@
         <v>87</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>87</v>
+        <v>407</v>
       </c>
       <c r="D118" s="21" t="s">
         <v>87</v>
@@ -4526,7 +4943,7 @@
         <v>286</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>286</v>
+        <v>408</v>
       </c>
       <c r="D119" s="21" t="s">
         <v>286</v>
@@ -4546,7 +4963,7 @@
         <v>62</v>
       </c>
       <c r="C120" s="21" t="s">
-        <v>62</v>
+        <v>409</v>
       </c>
       <c r="D120" s="21" t="s">
         <v>62</v>
@@ -4566,7 +4983,7 @@
         <v>20</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>20</v>
+        <v>410</v>
       </c>
       <c r="D121" s="21" t="s">
         <v>20</v>
@@ -4586,7 +5003,7 @@
         <v>287</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>287</v>
+        <v>411</v>
       </c>
       <c r="D122" s="21" t="s">
         <v>287</v>
@@ -4606,7 +5023,7 @@
         <v>39</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>39</v>
+        <v>412</v>
       </c>
       <c r="D123" s="21" t="s">
         <v>39</v>
@@ -4626,7 +5043,7 @@
         <v>114</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>114</v>
+        <v>413</v>
       </c>
       <c r="D124" s="21" t="s">
         <v>114</v>
@@ -4646,7 +5063,7 @@
         <v>46</v>
       </c>
       <c r="C125" s="21" t="s">
-        <v>46</v>
+        <v>414</v>
       </c>
       <c r="D125" s="21" t="s">
         <v>46</v>
@@ -4666,7 +5083,7 @@
         <v>109</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>109</v>
+        <v>415</v>
       </c>
       <c r="D126" s="21" t="s">
         <v>109</v>
@@ -4686,7 +5103,7 @@
         <v>288</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>288</v>
+        <v>416</v>
       </c>
       <c r="D127" s="21" t="s">
         <v>288</v>
@@ -4706,7 +5123,7 @@
         <v>49</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>49</v>
+        <v>417</v>
       </c>
       <c r="D128" s="21" t="s">
         <v>49</v>
@@ -4726,7 +5143,7 @@
         <v>58</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>58</v>
+        <v>418</v>
       </c>
       <c r="D129" s="21" t="s">
         <v>58</v>
@@ -4746,7 +5163,7 @@
         <v>38</v>
       </c>
       <c r="C130" s="21" t="s">
-        <v>38</v>
+        <v>419</v>
       </c>
       <c r="D130" s="21" t="s">
         <v>38</v>
@@ -4766,7 +5183,7 @@
         <v>74</v>
       </c>
       <c r="C131" s="21" t="s">
-        <v>74</v>
+        <v>420</v>
       </c>
       <c r="D131" s="21" t="s">
         <v>74</v>
@@ -4786,7 +5203,7 @@
         <v>124</v>
       </c>
       <c r="C132" s="21" t="s">
-        <v>124</v>
+        <v>421</v>
       </c>
       <c r="D132" s="21" t="s">
         <v>124</v>
@@ -4806,7 +5223,7 @@
         <v>98</v>
       </c>
       <c r="C133" s="21" t="s">
-        <v>98</v>
+        <v>422</v>
       </c>
       <c r="D133" s="21" t="s">
         <v>98</v>
@@ -4826,7 +5243,7 @@
         <v>26</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>26</v>
+        <v>423</v>
       </c>
       <c r="D134" s="21" t="s">
         <v>26</v>
@@ -4846,7 +5263,7 @@
         <v>91</v>
       </c>
       <c r="C135" s="22" t="s">
-        <v>91</v>
+        <v>424</v>
       </c>
       <c r="D135" s="22" t="s">
         <v>91</v>
@@ -4866,7 +5283,7 @@
         <v>102</v>
       </c>
       <c r="C136" s="21" t="s">
-        <v>102</v>
+        <v>425</v>
       </c>
       <c r="D136" s="21" t="s">
         <v>102</v>
@@ -4886,7 +5303,7 @@
         <v>95</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>95</v>
+        <v>426</v>
       </c>
       <c r="D137" s="21" t="s">
         <v>95</v>
@@ -4906,7 +5323,7 @@
         <v>48</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>48</v>
+        <v>427</v>
       </c>
       <c r="D138" s="21" t="s">
         <v>48</v>
@@ -4926,7 +5343,7 @@
         <v>23</v>
       </c>
       <c r="C139" s="21" t="s">
-        <v>23</v>
+        <v>428</v>
       </c>
       <c r="D139" s="21" t="s">
         <v>23</v>
@@ -4946,7 +5363,7 @@
         <v>289</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>289</v>
+        <v>429</v>
       </c>
       <c r="D140" s="21" t="s">
         <v>289</v>

</xml_diff>

<commit_message>
implements deleteTool at v-chip level and at v-select change event
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74941AC1-BAE5-B141-8AF7-989E95D70D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132F1C3-0F77-F244-9E9D-DB01B3A9D6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21100" yWindow="500" windowWidth="25800" windowHeight="26720" activeTab="2" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
+    <workbookView xWindow="11540" yWindow="500" windowWidth="32920" windowHeight="22080" activeTab="8" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="12" r:id="rId1"/>
@@ -2564,7 +2564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95BFF06-8D57-49C9-8C64-072E2F5A5508}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -5867,8 +5867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871C91-0278-42EA-88A7-88F9AAA1702C}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5904,7 +5904,7 @@
         <v>196</v>
       </c>
       <c r="D2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
coass de formateo de texto en titulos para que quepan style="word-break: break-word"
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3033B0C9-B5B1-4740-926A-E06ADBD46116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E671D4DC-C173-2346-9C81-36C3C3B58827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="500" windowWidth="29120" windowHeight="18240" firstSheet="1" activeTab="8" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="4480" yWindow="500" windowWidth="29120" windowHeight="18240" firstSheet="1" activeTab="9" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -1149,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D787E12B-D605-4928-A0CC-8A4E7610017F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1356,7 +1356,7 @@
     <col min="4" max="4" width="33.5" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="7" max="7" width="80.1640625" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
@@ -3803,7 +3803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E487C1-7907-4E12-B779-39278A63ADAD}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adds Narrative Topics data upload logic, and all changes to take into account the id_topic in table Narrative and AddNarrative component
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingrid.valero\OneDrive - FINAC S.A.S\Documents\Enviado por LG\Domeq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129722F8-53E2-437C-8222-7D7C6B565B0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BB9237-7768-6648-B58C-41FBC8CCD404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="495" windowWidth="29115" windowHeight="18240" firstSheet="5" activeTab="6" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="9580" yWindow="12200" windowWidth="39500" windowHeight="14420" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Posibles_rtas" sheetId="9" r:id="rId10"/>
     <sheet name="Preguntas" sheetId="10" r:id="rId11"/>
     <sheet name="Preg-NetworkMode" sheetId="11" r:id="rId12"/>
+    <sheet name="Narrativas_topicos" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Nodes!$A$1:$G$34</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="216">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -654,13 +655,46 @@
   </si>
   <si>
     <t>[{"texto":"Ninguna", "valor":0 },{"texto":"Lo ejecuto","valor":1 },{"texto":"Le envío información", "valor":2},{"texto":"Uso el resultado", "valor":3}]</t>
+  </si>
+  <si>
+    <t>topic_es</t>
+  </si>
+  <si>
+    <t>topic_en</t>
+  </si>
+  <si>
+    <t>¿Qué se podría hacer desde el área administrativa, técnica y comercial para hacer más eficientes los resultados y procesos de su cargo y/o área?</t>
+  </si>
+  <si>
+    <t>¿Tiene idea de otras fuentes de información sobre las cuales podamos llegar a más clientes?</t>
+  </si>
+  <si>
+    <t>¿Conoce las implicaciones que tiene el no cuidar los recursos de conocimiento, financieros y físicos en los resultados de la empresa; qué observaciones tiene para optimizar estos recursos?</t>
+  </si>
+  <si>
+    <t>¿En términos de formación que temas considera debe fortalecer o adquirir para mejorar su desempeño?</t>
+  </si>
+  <si>
+    <t>¿Qué sugiere para mejorar la claridad en los pedidos de maquinaria, y la comunicación de la expectativa del cliente vs lo que estamos ofreciendo e instalando?</t>
+  </si>
+  <si>
+    <t>Narrativa</t>
+  </si>
+  <si>
+    <t>narrative</t>
+  </si>
+  <si>
+    <t>narrativa</t>
+  </si>
+  <si>
+    <t>Narrative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,13 +739,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -727,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -769,10 +823,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -789,9 +846,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,7 +886,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -935,7 +992,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,7 +1134,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1091,16 +1148,16 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -1145,19 +1202,19 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="130.7109375" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="130.6640625" customWidth="1"/>
+    <col min="3" max="3" width="79.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1191,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1205,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1219,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1233,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1247,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1261,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1275,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1289,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1303,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1317,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1340,25 +1397,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="80.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="80.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1390,7 +1447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1422,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1454,7 +1511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1486,7 +1543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1518,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1550,7 +1607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1582,7 +1639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1614,7 +1671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1646,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1678,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1704,7 +1761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1730,7 +1787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1762,7 +1819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1783,14 +1840,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" t="s">
         <v>202</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" t="s">
         <v>202</v>
       </c>
       <c r="H15" s="8" t="s">
@@ -1799,11 +1856,11 @@
       <c r="I15" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1823,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1843,7 +1900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1863,7 +1920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1883,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1903,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1923,7 +1980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1943,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1963,7 +2020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1983,7 +2040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2003,7 +2060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2023,7 +2080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2054,13 +2111,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -2068,7 +2125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2076,7 +2133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2084,7 +2141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2092,7 +2149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2100,7 +2157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2108,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2116,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2124,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2132,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2140,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2148,7 +2205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2156,7 +2213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2164,7 +2221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2172,7 +2229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2180,7 +2237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2188,7 +2245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2196,7 +2253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2204,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2212,7 +2269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2220,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2228,7 +2285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2236,7 +2293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2244,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2252,7 +2309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2260,7 +2317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2268,12 +2325,97 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C22E10-8F73-E742-A1D9-0D3C50C168A1}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="203.1640625" customWidth="1"/>
+    <col min="3" max="3" width="203.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2289,14 +2431,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2307,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2318,7 +2460,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2329,7 +2471,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2340,7 +2482,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2351,7 +2493,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2362,7 +2504,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2373,7 +2515,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2384,7 +2526,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2395,7 +2537,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2406,7 +2548,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2417,7 +2559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2441,16 +2583,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -2470,7 +2612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>145</v>
       </c>
@@ -2487,7 +2629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>163</v>
       </c>
@@ -2504,7 +2646,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>161</v>
       </c>
@@ -2533,21 +2675,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA62681-7E2B-4B35-BC8A-E80E4595026B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2564,7 +2706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2581,7 +2723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2598,7 +2740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2615,7 +2757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2632,7 +2774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2647,6 +2789,23 @@
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2656,18 +2815,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913923E1-7AD3-4169-8C27-23573B1FF763}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2675,7 +2834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2683,7 +2842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2691,7 +2850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2699,12 +2858,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2714,20 +2881,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701A4822-F862-4AEE-8F4B-3EA29CBFF0F2}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2738,7 +2905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2749,7 +2916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2760,7 +2927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2771,7 +2938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2782,7 +2949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2793,7 +2960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2802,6 +2969,17 @@
       </c>
       <c r="C7" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2813,22 +2991,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3A88F-AA65-4A26-9859-BBB38B053428}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" customWidth="1"/>
-    <col min="3" max="3" width="77.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" customWidth="1"/>
+    <col min="3" max="3" width="77.6640625" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="54.28515625" customWidth="1"/>
-    <col min="7" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="54.33203125" customWidth="1"/>
+    <col min="7" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2854,7 +3032,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2880,7 +3058,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2906,7 +3084,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2932,7 +3110,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2958,7 +3136,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2984,7 +3162,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3010,7 +3188,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3036,7 +3214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3062,7 +3240,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3088,7 +3266,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3114,7 +3292,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3140,7 +3318,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3166,7 +3344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3192,7 +3370,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3218,7 +3396,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3244,7 +3422,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3270,7 +3448,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3296,7 +3474,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3322,7 +3500,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3348,7 +3526,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3374,7 +3552,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3400,7 +3578,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3426,7 +3604,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3452,7 +3630,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3478,7 +3656,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3504,7 +3682,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3530,7 +3708,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3556,7 +3734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3582,7 +3760,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3608,7 +3786,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3634,7 +3812,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3660,7 +3838,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3686,7 +3864,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3726,13 +3904,13 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -3746,7 +3924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3760,7 +3938,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3774,7 +3952,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3795,21 +3973,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E487C1-7907-4E12-B779-39278A63ADAD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -3823,7 +4001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3835,7 +4013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3847,7 +4025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3859,7 +4037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3870,7 +4048,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -3881,7 +4059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -3892,7 +4070,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3901,6 +4079,17 @@
       </c>
       <c r="C8" s="13" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se actualiza la data de cargue para Domecq ....
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/domecq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BB9237-7768-6648-B58C-41FBC8CCD404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA816D8C-4A8E-974A-A788-C055C8E71BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="12200" windowWidth="39500" windowHeight="14420" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="480" yWindow="1340" windowWidth="20000" windowHeight="24560" firstSheet="7" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="226">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -93,21 +93,9 @@
     <t>bimodal</t>
   </si>
   <si>
-    <t>Recursos</t>
-  </si>
-  <si>
     <t>resource</t>
   </si>
   <si>
-    <t>explora</t>
-  </si>
-  <si>
-    <t>Recurso</t>
-  </si>
-  <si>
-    <t>DataWise</t>
-  </si>
-  <si>
     <t>id_node_segment</t>
   </si>
   <si>
@@ -657,25 +645,67 @@
     <t>[{"texto":"Ninguna", "valor":0 },{"texto":"Lo ejecuto","valor":1 },{"texto":"Le envío información", "valor":2},{"texto":"Uso el resultado", "valor":3}]</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>max_selections</t>
+  </si>
+  <si>
+    <t>Conocimientos de Herramientas</t>
+  </si>
+  <si>
     <t>topic_es</t>
   </si>
   <si>
     <t>topic_en</t>
   </si>
   <si>
-    <t>¿Qué se podría hacer desde el área administrativa, técnica y comercial para hacer más eficientes los resultados y procesos de su cargo y/o área?</t>
-  </si>
-  <si>
-    <t>¿Tiene idea de otras fuentes de información sobre las cuales podamos llegar a más clientes?</t>
-  </si>
-  <si>
-    <t>¿Conoce las implicaciones que tiene el no cuidar los recursos de conocimiento, financieros y físicos en los resultados de la empresa; qué observaciones tiene para optimizar estos recursos?</t>
-  </si>
-  <si>
-    <t>¿En términos de formación que temas considera debe fortalecer o adquirir para mejorar su desempeño?</t>
-  </si>
-  <si>
-    <t>¿Qué sugiere para mejorar la claridad en los pedidos de maquinaria, y la comunicación de la expectativa del cliente vs lo que estamos ofreciendo e instalando?</t>
+    <t>¿Qué propone para que el trabajo en equipo permita lograr entre todos los objetivos de la compañía?</t>
+  </si>
+  <si>
+    <t>¿Cuál es su propuesta para que el trabajo en equipo en la compañía permita mejorar la comunicación al interior de ella?</t>
+  </si>
+  <si>
+    <t>¿Qué estrategias propone para que el trabajo en equipo en la compañía permita mejorar la comunicación entre las diferentes áreas?</t>
+  </si>
+  <si>
+    <t>¿Qué sugerencias tiene para que el trabajo en equipo en la compañía permita lograr la mejora continua en nuestros procesos?</t>
+  </si>
+  <si>
+    <t>Siesa</t>
+  </si>
+  <si>
+    <t>Cuadro de control de producción</t>
+  </si>
+  <si>
+    <t>Inventarios de producto nacional</t>
+  </si>
+  <si>
+    <t>Cuadro de seguimiento de la venta</t>
+  </si>
+  <si>
+    <t>Cuadro seguimiento de facturas</t>
+  </si>
+  <si>
+    <t>Tablero físico de control</t>
+  </si>
+  <si>
+    <t>Panel de control operativo</t>
+  </si>
+  <si>
+    <t>Indicadores de seguimiento</t>
+  </si>
+  <si>
+    <t>UNOEE</t>
+  </si>
+  <si>
+    <t>Documento del área de operaciones</t>
+  </si>
+  <si>
+    <t>Herramientas</t>
+  </si>
+  <si>
+    <t>Consulta de procedimientos en la Intranet</t>
   </si>
   <si>
     <t>Narrativa</t>
@@ -694,7 +724,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,33 +769,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -781,7 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -823,10 +833,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1176,10 +1182,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2">
         <v>45352</v>
@@ -1199,190 +1205,197 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D787E12B-D605-4928-A0CC-8A4E7610017F}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="130.6640625" customWidth="1"/>
+    <col min="2" max="2" width="121.6640625" customWidth="1"/>
     <col min="3" max="3" width="79.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -1397,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1420,31 +1433,31 @@
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1452,28 +1465,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -1484,28 +1497,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1516,28 +1529,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1548,28 +1561,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -1580,28 +1593,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J6">
         <v>9</v>
@@ -1612,28 +1625,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J7">
         <v>9</v>
@@ -1644,28 +1657,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J8">
         <v>9</v>
@@ -1676,28 +1689,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J9">
         <v>7</v>
@@ -1708,28 +1721,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="F10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -1740,22 +1753,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J11">
         <v>11</v>
@@ -1766,22 +1779,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J12">
         <v>7</v>
@@ -1792,28 +1805,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J13">
         <v>8</v>
@@ -1824,17 +1837,17 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D14" s="8"/>
       <c r="H14" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -1845,16 +1858,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J15">
         <v>10</v>
@@ -1865,16 +1878,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1885,16 +1898,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J17">
         <v>6</v>
@@ -1905,16 +1918,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J18">
         <v>7</v>
@@ -1925,16 +1938,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J19">
         <v>4</v>
@@ -1945,16 +1958,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J20">
         <v>7</v>
@@ -1965,16 +1978,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J21">
         <v>7</v>
@@ -1985,16 +1998,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J22">
         <v>7</v>
@@ -2005,16 +2018,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J23">
         <v>4</v>
@@ -2025,16 +2038,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J24">
         <v>7</v>
@@ -2045,16 +2058,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J25">
         <v>4</v>
@@ -2065,16 +2078,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J26">
         <v>10</v>
@@ -2085,16 +2098,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J27">
         <v>9</v>
@@ -2109,7 +2122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA2059D-6C61-454C-A9B8-08A3C88D6682}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2119,10 +2134,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2339,83 +2354,71 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C22E10-8F73-E742-A1D9-0D3C50C168A1}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3042CE92-63A8-44A4-B4EF-831678C97DF5}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="203.1640625" customWidth="1"/>
-    <col min="3" max="3" width="203.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="120.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C5" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2454,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2465,10 +2468,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2476,10 +2479,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2487,10 +2490,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2498,10 +2501,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2509,10 +2512,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2520,10 +2523,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2531,10 +2534,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2542,10 +2545,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2553,10 +2556,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2564,10 +2567,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2614,53 +2617,53 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E2">
         <v>3456435</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E3">
         <v>4563456</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E4">
         <v>35673</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2678,7 +2681,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2728,13 +2731,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -2745,13 +2748,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -2762,13 +2765,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -2779,16 +2782,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2796,16 +2799,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2815,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913923E1-7AD3-4169-8C27-23573B1FF763}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2847,7 +2850,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2855,23 +2858,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2881,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701A4822-F862-4AEE-8F4B-3EA29CBFF0F2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2896,13 +2883,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,10 +2908,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2932,10 +2919,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2943,10 +2930,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2954,10 +2941,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2965,21 +2952,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C8" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2989,10 +2965,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3A88F-AA65-4A26-9859-BBB38B053428}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3017,19 +2993,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3037,25 +3013,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3063,25 +3039,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3089,25 +3065,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3115,25 +3091,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3141,25 +3117,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3167,25 +3143,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3193,25 +3169,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3219,25 +3195,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3245,25 +3221,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3271,25 +3247,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3297,25 +3273,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3323,25 +3299,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3349,25 +3325,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -3375,25 +3351,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3401,25 +3377,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -3427,25 +3403,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3453,25 +3429,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -3479,25 +3455,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -3505,25 +3481,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3531,25 +3507,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3557,25 +3533,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -3583,25 +3559,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -3609,25 +3585,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -3635,25 +3611,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -3661,25 +3637,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3687,25 +3663,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -3713,25 +3689,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -3739,25 +3715,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F29" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3765,25 +3741,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3791,25 +3767,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C31" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3817,25 +3793,25 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C32" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -3843,25 +3819,25 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -3869,25 +3845,311 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>210</v>
+      </c>
+      <c r="C35" t="s">
+        <v>210</v>
+      </c>
+      <c r="D35" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" t="s">
+        <v>220</v>
+      </c>
+      <c r="F35" t="s">
+        <v>220</v>
+      </c>
+      <c r="G35" t="s">
         <v>77</v>
       </c>
-      <c r="E34" t="s">
-        <v>134</v>
-      </c>
-      <c r="F34" t="s">
-        <v>134</v>
-      </c>
-      <c r="G34" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" t="s">
-        <v>90</v>
+      <c r="H35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E36" t="s">
+        <v>220</v>
+      </c>
+      <c r="F36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" t="s">
+        <v>220</v>
+      </c>
+      <c r="F37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" t="s">
+        <v>220</v>
+      </c>
+      <c r="F38" t="s">
+        <v>220</v>
+      </c>
+      <c r="G38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" t="s">
+        <v>203</v>
+      </c>
+      <c r="E39" t="s">
+        <v>220</v>
+      </c>
+      <c r="F39" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40" t="s">
+        <v>215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>203</v>
+      </c>
+      <c r="E40" t="s">
+        <v>220</v>
+      </c>
+      <c r="F40" t="s">
+        <v>220</v>
+      </c>
+      <c r="G40" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41" t="s">
+        <v>216</v>
+      </c>
+      <c r="D41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E41" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" t="s">
+        <v>217</v>
+      </c>
+      <c r="D42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" t="s">
+        <v>220</v>
+      </c>
+      <c r="F42" t="s">
+        <v>220</v>
+      </c>
+      <c r="G42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>218</v>
+      </c>
+      <c r="C43" t="s">
+        <v>218</v>
+      </c>
+      <c r="D43" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" t="s">
+        <v>219</v>
+      </c>
+      <c r="D44" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" t="s">
+        <v>220</v>
+      </c>
+      <c r="G44" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>221</v>
+      </c>
+      <c r="C45" t="s">
+        <v>221</v>
+      </c>
+      <c r="D45" t="s">
+        <v>203</v>
+      </c>
+      <c r="E45" t="s">
+        <v>220</v>
+      </c>
+      <c r="F45" t="s">
+        <v>220</v>
+      </c>
+      <c r="G45" t="s">
+        <v>82</v>
+      </c>
+      <c r="H45" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3929,13 +4191,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3943,13 +4205,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3957,13 +4219,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3976,7 +4238,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3992,13 +4254,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4010,7 +4272,7 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4022,7 +4284,7 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4034,7 +4296,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4042,10 +4304,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4053,10 +4315,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4064,10 +4326,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4075,10 +4337,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>17</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4086,10 +4348,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se cambia el  archivo IRA_DATA para cargue de modelos preguntas etc
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/domecq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA816D8C-4A8E-974A-A788-C055C8E71BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2760B-D6D9-614A-9360-6BDED7943E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1340" windowWidth="20000" windowHeight="24560" firstSheet="7" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="4480" yWindow="1600" windowWidth="29120" windowHeight="18240" firstSheet="2" activeTab="8" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="230">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -93,9 +93,6 @@
     <t>bimodal</t>
   </si>
   <si>
-    <t>resource</t>
-  </si>
-  <si>
     <t>id_node_segment</t>
   </si>
   <si>
@@ -177,24 +174,6 @@
     <t>creativethink</t>
   </si>
   <si>
-    <t>¿A quién acude cuando tiene un problema con un cliente?</t>
-  </si>
-  <si>
-    <t>¿A quién acude cuando tiene un problema con un compañero de trabajo?</t>
-  </si>
-  <si>
-    <t>¿A quién acude para discutir temas de desarrollo personal/profesional?</t>
-  </si>
-  <si>
-    <t>¿De quién recibe información útil para desarrollar su trabajo?</t>
-  </si>
-  <si>
-    <t>¿Con quién desarrolla trabajo en equipo?</t>
-  </si>
-  <si>
-    <t>¿Qué tanto conozco las competencias y conocimentos que esta persona tiene?</t>
-  </si>
-  <si>
     <t>¿En caso de ausencia temporal suya a quién se puede acudir para resolver algo que sea de su responsabilidad?</t>
   </si>
   <si>
@@ -222,9 +201,6 @@
     <t>Trabajo en equipo</t>
   </si>
   <si>
-    <t>Competencias y conocimientos</t>
-  </si>
-  <si>
     <t>Ausencia temporal</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
     <t>Acudo a esta persona por dificultades o conocimiento</t>
   </si>
   <si>
-    <t>¿A quién provee información útil para el desarrollo del trabajo?</t>
-  </si>
-  <si>
     <t>¿En el último año, he tenido reuniones con esta persona sobre ideas novedosas y/o creativas relacionada con la actividad de la compañía por estas razones?</t>
   </si>
   <si>
@@ -321,18 +294,6 @@
     <t>Puede seleccionar más de una razón.</t>
   </si>
   <si>
-    <t>Pueden ser conflictos por temas administrativos. Puede seleccionar más de una razón.</t>
-  </si>
-  <si>
-    <t>No incluir el acompañamiento para soluciones de problemas.</t>
-  </si>
-  <si>
-    <t>Puede incluir acompañamiento a solución de problemas.</t>
-  </si>
-  <si>
-    <t>Esto no quiere decir que yo tengo esos conocimientos y competencias, pero sí que identifico los conocimientos y competencias que esta persona tiene.</t>
-  </si>
-  <si>
     <t>marzo-2024</t>
   </si>
   <si>
@@ -480,9 +441,6 @@
     <t>[{"texto":"Nunca", "valor":0 },{"texto":"Diariamente", "valor":1 },{"texto":"Semanalmente", "valor":2},{"texto":"Mensualmente", "valor":3},{"texto":"Otro", "valor":4}]</t>
   </si>
   <si>
-    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por autoridad", "valor":2},{"texto":"Por creatividad", "valor":3}]</t>
-  </si>
-  <si>
     <t>[{"texto":"No", "valor":0 },{"texto":"Sí", "valor":1 },{"texto":"No sé", "valor":2}]</t>
   </si>
   <si>
@@ -660,18 +618,6 @@
     <t>topic_en</t>
   </si>
   <si>
-    <t>¿Qué propone para que el trabajo en equipo permita lograr entre todos los objetivos de la compañía?</t>
-  </si>
-  <si>
-    <t>¿Cuál es su propuesta para que el trabajo en equipo en la compañía permita mejorar la comunicación al interior de ella?</t>
-  </si>
-  <si>
-    <t>¿Qué estrategias propone para que el trabajo en equipo en la compañía permita mejorar la comunicación entre las diferentes áreas?</t>
-  </si>
-  <si>
-    <t>¿Qué sugerencias tiene para que el trabajo en equipo en la compañía permita lograr la mejora continua en nuestros procesos?</t>
-  </si>
-  <si>
     <t>Siesa</t>
   </si>
   <si>
@@ -708,16 +654,82 @@
     <t>Consulta de procedimientos en la Intranet</t>
   </si>
   <si>
+    <t>¿De quién recibe información útil para desarrollar su trabajo y con qué frecuencia?</t>
+  </si>
+  <si>
+    <t>No incluir el acompañamiento para soluciones de problemas, ni incluir reuniones formales periódicas.</t>
+  </si>
+  <si>
+    <t>¿A quién provee información útil para el desarrollo del trabajo y con qué frecuencia?</t>
+  </si>
+  <si>
+    <t>¿A quién acudo cuando tiene un problema con un cliente y por qué razón?</t>
+  </si>
+  <si>
+    <t>¿A quién le gustaría acceder para adquirir conocimiento o discutir temas del negocio, pero por falta de acceso, inseguridad o timidez no lo hace?</t>
+  </si>
+  <si>
+    <t>¿En el último año, he tenido reuniones con esta persona sobre ideas novedosas y/o creativas relacionada con la actividad de la compañía y por qué razón?</t>
+  </si>
+  <si>
+    <t>Una experiencia de trabajo en equipo que Usted ha identificado en la compañía en el último año y que considera que ha sido exitosa. Cuente por qué le pareció exitosa y qué se podría aprender de esa experiencia para aplicar en otras situaciones de la empresa. Si Usted participó en esa experiencia cuéntenos sobre su participación y cómo se sintió. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
+  </si>
+  <si>
+    <t>Una situación que Usted ha observado, que haya tenido dificultades y que esas dificultades hubieran sido menores si hubiera existido mejor comunicación y coordinación de tareas entre áreas. Trate de explicar cuáles fueron las dificultades en comunicación y coordinación, y en lo posible sugiera cómo estas cosas hubieran podido ser mejores. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
+  </si>
+  <si>
+    <t>¿Con quién desarrolla trabajo en equipo y con qué frecuencia?</t>
+  </si>
+  <si>
+    <t>Incluya el acompañamiento a solución de problemas, pero no incluir reuniones formales periódicas.</t>
+  </si>
+  <si>
+    <t>¿A quién acude cuando tiene un problema con un compañero de trabajo y por qué razón?</t>
+  </si>
+  <si>
+    <t>Puede ser por temas administrativos. Puede seleccionar más de una razón.</t>
+  </si>
+  <si>
+    <t>¿A quién acude para discutir temas de desarrollo personal/profesional y por qué razón?</t>
+  </si>
+  <si>
+    <t>Es búsqueda de ayuda para definir cómo resolver alguna dificultad o desconocimiento que le está impidiendo realizar una tarea. Puede seleccionar más de una razón.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indique las razones por las cuales quisiera acceder a esa persona. </t>
+  </si>
+  <si>
+    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por conocimiento", "valor":2},{"texto":"Por creatividad", "valor":3},{"texto":"Por jerarquía", "valor":4},{"texto":"Por buena energía", "valor":5}]</t>
+  </si>
+  <si>
+    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por conducto regular ", "valor":2},{"texto":"Por creatividad", "valor":3},{"texto":"Por jerarquía", "valor":4},{"texto":"Por buena energía", "valor":5}]</t>
+  </si>
+  <si>
+    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por conocimiento", "valor":2},{"texto":"Por creatividad", "valor":3},{"texto":"Por buena energía", "valor":4}]</t>
+  </si>
+  <si>
+    <t>Acceder para adquirir conocimiento</t>
+  </si>
+  <si>
+    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por conocimiento", "valor":2},{"texto":"Por creatividad", "valor":3},{"texto":"Por influencia", "valor":4},{"texto":"Por buena energía", "valor":5}]</t>
+  </si>
+  <si>
+    <t>[{"texto":"Por experiencia", "valor":0 },{"texto":"Por confianza", "valor":1 },{"texto":"Por conocimiento", "valor":2},{"texto":"Por creatividad", "valor":3},{"texto":"Por jerarquía", "valor":4}]</t>
+  </si>
+  <si>
+    <t>[{"texto":"Ninguna", "valor":0 },{"texto":"Lo ejecuto","valor":1 },{"texto":"Le envío información", "valor":2},{"texto":"Uso el resultado", "valor":3},{"texto":"Dependo de su ejecución", "valor":4}]</t>
+  </si>
+  <si>
+    <t>narrative</t>
+  </si>
+  <si>
+    <t>Narrative</t>
+  </si>
+  <si>
     <t>Narrativa</t>
   </si>
   <si>
-    <t>narrative</t>
-  </si>
-  <si>
     <t>narrativa</t>
-  </si>
-  <si>
-    <t>Narrative</t>
   </si>
 </sst>
 </file>
@@ -824,15 +836,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,10 +1194,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2">
         <v>45352</v>
@@ -1205,16 +1217,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D787E12B-D605-4928-A0CC-8A4E7610017F}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="121.6640625" customWidth="1"/>
+    <col min="2" max="2" width="172.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1226,25 +1238,25 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="H1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1252,10 +1264,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -1266,10 +1278,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1280,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1294,10 +1306,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1308,10 +1320,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1322,10 +1334,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1336,10 +1348,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1350,10 +1362,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -1364,10 +1376,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1378,10 +1390,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1392,12 +1404,68 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1410,19 +1478,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="82.33203125" customWidth="1"/>
     <col min="3" max="3" width="40.83203125" customWidth="1"/>
     <col min="4" max="4" width="33.5" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" customWidth="1"/>
-    <col min="7" max="7" width="80.1640625" customWidth="1"/>
+    <col min="7" max="7" width="38" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
@@ -1433,31 +1501,31 @@
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1465,28 +1533,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -1497,31 +1565,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>215</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>215</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1529,28 +1597,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>47</v>
+        <v>216</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>47</v>
+        <v>216</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1561,31 +1629,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1593,28 +1661,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="J6">
         <v>9</v>
@@ -1625,28 +1693,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J7">
         <v>9</v>
@@ -1657,28 +1725,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>49</v>
+        <v>212</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>212</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>213</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>213</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J8">
         <v>9</v>
@@ -1686,444 +1754,445 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J10">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J11">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" t="s">
-        <v>92</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="J13">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>184</v>
+      </c>
       <c r="H14" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J14">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" t="s">
-        <v>198</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J15">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>199</v>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J17">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>196</v>
+        <v>61</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>196</v>
+        <v>61</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J18">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>195</v>
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" t="s">
+        <v>182</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>196</v>
-      </c>
-      <c r="C21" t="s">
-        <v>196</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J21">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>197</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J22">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>70</v>
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>181</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J24">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>193</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>193</v>
+        <v>79</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J25">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J26">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>208</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>208</v>
+      </c>
+      <c r="D27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F27" t="s">
+        <v>218</v>
+      </c>
+      <c r="G27" t="s">
+        <v>218</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="J27">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA2059D-6C61-454C-A9B8-08A3C88D6682}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2134,10 +2203,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2198,7 +2267,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2206,15 +2275,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2222,7 +2291,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2230,15 +2299,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2246,7 +2315,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -2254,7 +2323,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2262,7 +2331,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -2270,7 +2339,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2278,15 +2347,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -2294,7 +2363,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -2302,7 +2371,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -2310,15 +2379,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -2326,26 +2395,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2355,15 +2408,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3042CE92-63A8-44A4-B4EF-831678C97DF5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="120.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2371,10 +2426,10 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2382,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2393,32 +2448,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2457,10 +2490,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2468,10 +2501,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2479,10 +2512,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2490,10 +2523,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2501,10 +2534,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2512,10 +2545,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2523,10 +2556,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2534,10 +2567,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2545,10 +2578,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2556,10 +2589,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2567,10 +2600,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2617,53 +2650,53 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>140</v>
+        <v>126</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="E2">
         <v>3456435</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>158</v>
+        <v>129</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="E3">
         <v>4563456</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>156</v>
+        <v>141</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="E4">
         <v>35673</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2678,10 +2711,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA62681-7E2B-4B35-BC8A-E80E4595026B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2731,13 +2764,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -2748,13 +2781,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -2765,13 +2798,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -2782,33 +2815,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>226</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C7" t="s">
-        <v>222</v>
-      </c>
-      <c r="D7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E7" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2821,7 +2837,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2850,7 +2866,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2858,7 +2874,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2868,10 +2884,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701A4822-F862-4AEE-8F4B-3EA29CBFF0F2}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2883,13 +2899,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2908,10 +2924,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2919,10 +2935,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2930,32 +2946,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>203</v>
+      <c r="B6" t="s">
+        <v>227</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2967,7 +2972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3A88F-AA65-4A26-9859-BBB38B053428}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -2993,19 +2998,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3013,25 +3018,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3039,25 +3044,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3065,25 +3070,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3091,25 +3096,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3117,25 +3122,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3143,25 +3148,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
         <v>71</v>
       </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3169,25 +3174,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3195,25 +3200,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3221,25 +3226,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3247,25 +3252,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3273,25 +3278,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3299,25 +3304,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3325,25 +3330,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -3351,25 +3356,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3377,25 +3382,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -3403,25 +3408,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3429,25 +3434,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -3455,25 +3460,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -3481,25 +3486,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3507,25 +3512,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3533,25 +3538,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -3559,25 +3564,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -3585,25 +3590,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F24" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -3611,25 +3616,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -3637,25 +3642,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3663,25 +3668,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -3689,25 +3694,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -3715,25 +3720,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3741,25 +3746,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H30" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3767,25 +3772,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3793,25 +3798,25 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C32" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F32" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -3819,25 +3824,25 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -3845,25 +3850,25 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="F34" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G34" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3871,25 +3876,25 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C35" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E35" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F35" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -3897,25 +3902,25 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="C36" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="D36" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E36" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F36" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G36" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -3923,25 +3928,25 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C37" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D37" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E37" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F37" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G37" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -3949,25 +3954,25 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C38" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F38" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G38" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -3975,25 +3980,25 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C39" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D39" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E39" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F39" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G39" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H39" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -4001,25 +4006,25 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E40" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F40" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -4027,25 +4032,25 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C41" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E41" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F41" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G41" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H41" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -4053,25 +4058,25 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="C42" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="D42" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E42" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F42" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G42" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H42" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -4079,25 +4084,25 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F43" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -4105,25 +4110,25 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="C44" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E44" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F44" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -4131,25 +4136,25 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="C45" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D45" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E45" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F45" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G45" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H45" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4191,13 +4196,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4205,13 +4210,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4219,13 +4224,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4235,10 +4240,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E487C1-7907-4E12-B779-39278A63ADAD}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4254,13 +4259,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4272,7 +4277,7 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4284,7 +4289,7 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4296,7 +4301,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,10 +4309,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4315,10 +4320,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4326,10 +4331,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4337,21 +4342,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se completa la plantilla de IRA_data
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingrid.valero\OneDrive - FINAC S.A.S\Documents\Formularios_OIHUB\DOMECQ\Plantillas_oficiales_cargue_DOMECQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2760B-D6D9-614A-9360-6BDED7943E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7C78EA-0365-44CD-8801-A3703A0E5E5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="1600" windowWidth="29120" windowHeight="18240" firstSheet="2" activeTab="8" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="4485" yWindow="495" windowWidth="29115" windowHeight="18240" firstSheet="4" activeTab="6" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="231">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -93,6 +93,9 @@
     <t>bimodal</t>
   </si>
   <si>
+    <t>resource</t>
+  </si>
+  <si>
     <t>id_node_segment</t>
   </si>
   <si>
@@ -609,9 +612,6 @@
     <t>max_selections</t>
   </si>
   <si>
-    <t>Conocimientos de Herramientas</t>
-  </si>
-  <si>
     <t>topic_es</t>
   </si>
   <si>
@@ -648,9 +648,6 @@
     <t>Documento del área de operaciones</t>
   </si>
   <si>
-    <t>Herramientas</t>
-  </si>
-  <si>
     <t>Consulta de procedimientos en la Intranet</t>
   </si>
   <si>
@@ -720,16 +717,22 @@
     <t>[{"texto":"Ninguna", "valor":0 },{"texto":"Lo ejecuto","valor":1 },{"texto":"Le envío información", "valor":2},{"texto":"Uso el resultado", "valor":3},{"texto":"Dependo de su ejecución", "valor":4}]</t>
   </si>
   <si>
+    <t>Uso de Recursos</t>
+  </si>
+  <si>
+    <t>Narrativa</t>
+  </si>
+  <si>
     <t>narrative</t>
   </si>
   <si>
+    <t>narrativa</t>
+  </si>
+  <si>
     <t>Narrative</t>
   </si>
   <si>
-    <t>Narrativa</t>
-  </si>
-  <si>
-    <t>narrativa</t>
+    <t>Recursos</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -842,12 +845,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -864,9 +866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -904,7 +906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1010,7 +1012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1152,7 +1154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1166,16 +1168,16 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1192,12 +1194,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2">
         <v>45352</v>
@@ -1220,250 +1222,250 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="172.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="172.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -1478,704 +1480,704 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" customWidth="1"/>
-    <col min="2" max="2" width="82.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="G3" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" t="s">
-        <v>215</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="F5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="J5">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
         <v>204</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="G6" t="s">
         <v>204</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>205</v>
-      </c>
-      <c r="G6" t="s">
-        <v>205</v>
-      </c>
       <c r="H6" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="G8" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G8" t="s">
-        <v>213</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J10">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" t="s">
-        <v>184</v>
+      <c r="B14" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14">
+        <v>82</v>
+      </c>
+      <c r="J14" s="16">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J18">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J21">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J27">
         <v>14</v>
@@ -2189,27 +2191,27 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA2059D-6C61-454C-A9B8-08A3C88D6682}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2217,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2225,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2249,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2257,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2273,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2297,7 +2299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -2305,7 +2307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -2313,7 +2315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -2321,7 +2323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -2353,7 +2355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2369,7 +2371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -2377,7 +2379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -2393,11 +2395,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>27</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>2</v>
       </c>
     </row>
@@ -2410,18 +2428,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3042CE92-63A8-44A4-B4EF-831678C97DF5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.6640625" customWidth="1"/>
+    <col min="2" max="2" width="79.5703125" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2432,26 +2449,26 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2467,14 +2484,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2485,125 +2502,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2619,16 +2636,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -2648,55 +2665,55 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="E2">
         <v>3456435</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>144</v>
       </c>
       <c r="E3">
         <v>4563456</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>142</v>
       </c>
       <c r="E4">
         <v>35673</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2711,21 +2728,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA62681-7E2B-4B35-BC8A-E80E4595026B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2742,7 +2760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2759,72 +2777,89 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" t="s">
         <v>228</v>
-      </c>
-      <c r="C6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D6" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2837,15 +2872,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2853,7 +2888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2861,20 +2896,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2884,31 +2919,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701A4822-F862-4AEE-8F4B-3EA29CBFF0F2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2919,48 +2954,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2972,22 +3018,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3A88F-AA65-4A26-9859-BBB38B053428}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="91.1640625" customWidth="1"/>
-    <col min="3" max="3" width="77.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
-    <col min="6" max="6" width="54.33203125" customWidth="1"/>
-    <col min="7" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="6" max="6" width="54.28515625" customWidth="1"/>
+    <col min="7" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -2998,880 +3044,880 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3882,22 +3928,22 @@
         <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E35" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3908,22 +3954,22 @@
         <v>193</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E36" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F36" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3934,22 +3980,22 @@
         <v>194</v>
       </c>
       <c r="D37" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E37" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F37" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3960,22 +4006,22 @@
         <v>195</v>
       </c>
       <c r="D38" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F38" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3986,22 +4032,22 @@
         <v>196</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E39" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F39" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4012,22 +4058,22 @@
         <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E40" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F40" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4038,22 +4084,22 @@
         <v>198</v>
       </c>
       <c r="D41" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E41" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G41" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4064,22 +4110,22 @@
         <v>199</v>
       </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E42" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G42" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4090,22 +4136,22 @@
         <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F43" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4116,45 +4162,45 @@
         <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F44" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>203</v>
-      </c>
-      <c r="C45" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>202</v>
       </c>
       <c r="D45" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="F45" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -4168,16 +4214,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -4191,46 +4237,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4240,35 +4286,35 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E487C1-7907-4E12-B779-39278A63ADAD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -4277,10 +4323,10 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -4289,10 +4335,10 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -4301,51 +4347,62 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>227</v>
+      </c>
+      <c r="C9" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevos cambios de docmecq solictados en textos de narratoivas , campo titulo no obligatrio en narrativas
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A5E8C5-A93D-6F4D-BC0F-FC715C2E1CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA50629-8E96-5A46-98B1-F4EFA1B5CFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15740" yWindow="2580" windowWidth="33440" windowHeight="18760" activeTab="2" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="22100" yWindow="11020" windowWidth="39120" windowHeight="23400" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="512">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -463,12 +463,6 @@
     <t>¿En el último año, he tenido reuniones con esta persona sobre ideas novedosas y/o creativas relacionada con la actividad de la compañía y por qué razón?</t>
   </si>
   <si>
-    <t>Una experiencia de trabajo en equipo que Usted ha identificado en la compañía en el último año y que considera que ha sido exitosa. Cuente por qué le pareció exitosa y qué se podría aprender de esa experiencia para aplicar en otras situaciones de la empresa. Si Usted participó en esa experiencia cuéntenos sobre su participación y cómo se sintió. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
-  </si>
-  <si>
-    <t>Una situación que Usted ha observado, que haya tenido dificultades y que esas dificultades hubieran sido menores si hubiera existido mejor comunicación y coordinación de tareas entre áreas. Trate de explicar cuáles fueron las dificultades en comunicación y coordinación, y en lo posible sugiera cómo estas cosas hubieran podido ser mejores. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
-  </si>
-  <si>
     <t>¿Con quién desarrolla trabajo en equipo y con qué frecuencia?</t>
   </si>
   <si>
@@ -1577,6 +1571,12 @@
   </si>
   <si>
     <t>TESTTER</t>
+  </si>
+  <si>
+    <t>NARRATIVA 1: Una experiencia de trabajo en equipo que Usted ha identificado en la compañía en el último año y que considera que ha sido exitosa. Cuente por qué le pareció exitosa y qué se podría aprender de esa experiencia para aplicar en otras situaciones de la empresa. Si Usted participó en esa experiencia cuéntenos sobre su participación y cómo se sintió. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
+  </si>
+  <si>
+    <t>NARRATIVA 2: Una situación que Usted ha observado, que haya tenido dificultades y que esas dificultades hubieran sido menores si hubiera existido mejor comunicación y coordinación de tareas entre áreas. Trate de explicar cuáles fueron las dificultades en comunicación y coordinación, y en lo posible sugiera cómo estas cosas hubieran podido ser mejores. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
   </si>
 </sst>
 </file>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" s="18">
         <v>45444</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -2131,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2145,10 +2145,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2285,10 +2285,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -2299,10 +2299,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -2313,10 +2313,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -2327,10 +2327,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -2346,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CD784-6851-47BB-9FB9-9AB3A8D39F8B}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2433,10 +2433,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>48</v>
@@ -2445,10 +2445,10 @@
         <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>57</v>
@@ -2465,10 +2465,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>49</v>
@@ -2509,10 +2509,10 @@
         <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>57</v>
@@ -2593,10 +2593,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>52</v>
@@ -2605,10 +2605,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>57</v>
@@ -2741,10 +2741,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>76</v>
@@ -2781,10 +2787,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>76</v>
@@ -2841,10 +2847,10 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C18" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>76</v>
@@ -2861,10 +2867,10 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>76</v>
@@ -2927,16 +2933,16 @@
         <v>138</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>57</v>
@@ -3154,8 +3160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3042CE92-63A8-44A4-B4EF-831678C97DF5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3180,10 +3186,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>510</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3191,10 +3197,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>511</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -3234,10 +3240,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3245,10 +3251,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3256,10 +3262,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3300,10 +3306,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3333,10 +3339,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3355,10 +3361,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3388,10 +3394,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3404,7 +3410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C248DF4-33E4-45F0-A9B3-DCFFCEC7ACF1}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
@@ -3441,13 +3447,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3458,22 +3464,22 @@
         <v>29545232</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E2">
         <v>29545232</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2">
         <v>80715371</v>
       </c>
       <c r="H2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I2" s="13">
         <v>43570</v>
@@ -3487,22 +3493,22 @@
         <v>31973387</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E3">
         <v>31973387</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G3">
         <v>29545232</v>
       </c>
       <c r="H3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I3" s="13">
         <v>37643</v>
@@ -3516,22 +3522,22 @@
         <v>52374980</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E4">
         <v>52374980</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G4">
         <v>80715371</v>
       </c>
       <c r="H4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I4" s="13">
         <v>41214</v>
@@ -3545,22 +3551,22 @@
         <v>19345653</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E5">
         <v>19345653</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G5">
         <v>19345653</v>
       </c>
       <c r="H5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I5" s="13">
         <v>29677</v>
@@ -3574,22 +3580,22 @@
         <v>1098741216</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E6">
         <v>1098741216</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G6">
         <v>80715371</v>
       </c>
       <c r="H6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I6" s="13">
         <v>44417</v>
@@ -3603,22 +3609,22 @@
         <v>1114831933</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E7">
         <v>1114831933</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G7">
         <v>1107055110</v>
       </c>
       <c r="H7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I7" s="13">
         <v>44789</v>
@@ -3632,22 +3638,22 @@
         <v>1148693650</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E8">
         <v>1148693650</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G8">
         <v>1107055110</v>
       </c>
       <c r="H8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I8" s="13">
         <v>44882</v>
@@ -3661,22 +3667,22 @@
         <v>1107055110</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E9">
         <v>1107055110</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G9">
         <v>29545232</v>
       </c>
       <c r="H9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I9" s="13">
         <v>41932</v>
@@ -3690,22 +3696,22 @@
         <v>1110547979</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E10">
         <v>1110547979</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G10">
         <v>29545232</v>
       </c>
       <c r="H10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I10" s="13">
         <v>44781</v>
@@ -3719,10 +3725,10 @@
         <v>53002399</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E11">
         <v>53002399</v>
@@ -3734,7 +3740,7 @@
         <v>46664942</v>
       </c>
       <c r="H11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I11" s="13">
         <v>44728</v>
@@ -3748,10 +3754,10 @@
         <v>46664942</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E12">
         <v>46664942</v>
@@ -3763,7 +3769,7 @@
         <v>80715371</v>
       </c>
       <c r="H12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I12" s="13">
         <v>44669</v>
@@ -3777,10 +3783,10 @@
         <v>1007403183</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E13">
         <v>1007403183</v>
@@ -3792,7 +3798,7 @@
         <v>1020753630</v>
       </c>
       <c r="H13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I13" s="13">
         <v>44797</v>
@@ -3806,10 +3812,10 @@
         <v>66924921</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E14">
         <v>66924921</v>
@@ -3821,7 +3827,7 @@
         <v>1020753630</v>
       </c>
       <c r="H14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I14" s="13">
         <v>35150</v>
@@ -3835,10 +3841,10 @@
         <v>1020753630</v>
       </c>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E15">
         <v>1020753630</v>
@@ -3850,7 +3856,7 @@
         <v>80715371</v>
       </c>
       <c r="H15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I15" s="13">
         <v>43185</v>
@@ -3864,10 +3870,10 @@
         <v>39543835</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E16">
         <v>39543835</v>
@@ -3879,7 +3885,7 @@
         <v>21022544</v>
       </c>
       <c r="H16" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I16" s="13">
         <v>34608</v>
@@ -3893,10 +3899,10 @@
         <v>1015446720</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E17">
         <v>1015446720</v>
@@ -3908,7 +3914,7 @@
         <v>21022544</v>
       </c>
       <c r="H17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I17" s="13">
         <v>44413</v>
@@ -3922,10 +3928,10 @@
         <v>1010195301</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E18">
         <v>1010195301</v>
@@ -3937,7 +3943,7 @@
         <v>21022544</v>
       </c>
       <c r="H18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I18" s="13">
         <v>45231</v>
@@ -3951,10 +3957,10 @@
         <v>1023980003</v>
       </c>
       <c r="C19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E19">
         <v>1023980003</v>
@@ -3966,7 +3972,7 @@
         <v>21022544</v>
       </c>
       <c r="H19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I19" s="13">
         <v>44683</v>
@@ -3980,10 +3986,10 @@
         <v>1001048912</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E20">
         <v>1001048912</v>
@@ -3995,7 +4001,7 @@
         <v>21022544</v>
       </c>
       <c r="H20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I20" s="13">
         <v>45335</v>
@@ -4009,10 +4015,10 @@
         <v>1005777544</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E21">
         <v>1005777544</v>
@@ -4024,7 +4030,7 @@
         <v>21022544</v>
       </c>
       <c r="H21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I21" s="13">
         <v>43577</v>
@@ -4038,10 +4044,10 @@
         <v>21022544</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E22">
         <v>21022544</v>
@@ -4053,7 +4059,7 @@
         <v>80715371</v>
       </c>
       <c r="H22" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I22" s="13">
         <v>35898</v>
@@ -4067,22 +4073,22 @@
         <v>80715371</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E23">
         <v>80715371</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G23">
         <v>19345653</v>
       </c>
       <c r="H23" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I23" s="13">
         <v>39121</v>
@@ -4096,22 +4102,22 @@
         <v>1032376982</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E24">
         <v>1032376982</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G24">
         <v>80715371</v>
       </c>
       <c r="H24" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I24" s="13">
         <v>38867</v>
@@ -4125,10 +4131,10 @@
         <v>73231242</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E25">
         <v>73231242</v>
@@ -4140,7 +4146,7 @@
         <v>1088241672</v>
       </c>
       <c r="H25" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I25" s="13">
         <v>39181</v>
@@ -4154,10 +4160,10 @@
         <v>1000332619</v>
       </c>
       <c r="C26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E26">
         <v>1000332619</v>
@@ -4169,7 +4175,7 @@
         <v>79876965</v>
       </c>
       <c r="H26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I26" s="13">
         <v>44652</v>
@@ -4183,10 +4189,10 @@
         <v>94384294</v>
       </c>
       <c r="C27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E27">
         <v>94384294</v>
@@ -4198,7 +4204,7 @@
         <v>1088241672</v>
       </c>
       <c r="H27" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I27" s="13">
         <v>35034</v>
@@ -4212,10 +4218,10 @@
         <v>80427593</v>
       </c>
       <c r="C28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E28">
         <v>80427593</v>
@@ -4227,7 +4233,7 @@
         <v>80715371</v>
       </c>
       <c r="H28" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I28" s="13">
         <v>35726</v>
@@ -4241,10 +4247,10 @@
         <v>1016945353</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E29">
         <v>1016945353</v>
@@ -4256,7 +4262,7 @@
         <v>79876965</v>
       </c>
       <c r="H29" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I29" s="13">
         <v>45314</v>
@@ -4270,10 +4276,10 @@
         <v>79876965</v>
       </c>
       <c r="C30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E30">
         <v>79876965</v>
@@ -4285,7 +4291,7 @@
         <v>80715371</v>
       </c>
       <c r="H30" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I30" s="13">
         <v>44636</v>
@@ -4299,10 +4305,10 @@
         <v>52328100</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E31">
         <v>52328100</v>
@@ -4314,7 +4320,7 @@
         <v>80427593</v>
       </c>
       <c r="H31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I31" s="13">
         <v>42461</v>
@@ -4328,10 +4334,10 @@
         <v>79979041</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E32">
         <v>79979041</v>
@@ -4343,7 +4349,7 @@
         <v>80427593</v>
       </c>
       <c r="H32" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I32" s="13">
         <v>43129</v>
@@ -4357,10 +4363,10 @@
         <v>1130618065</v>
       </c>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E33">
         <v>1130618065</v>
@@ -4372,7 +4378,7 @@
         <v>1088241672</v>
       </c>
       <c r="H33" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I33" s="13">
         <v>44882</v>
@@ -4386,10 +4392,10 @@
         <v>1033725996</v>
       </c>
       <c r="C34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E34">
         <v>1033725996</v>
@@ -4401,7 +4407,7 @@
         <v>79876965</v>
       </c>
       <c r="H34" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I34" s="13">
         <v>40043</v>
@@ -4415,10 +4421,10 @@
         <v>31588862</v>
       </c>
       <c r="C35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E35">
         <v>31588862</v>
@@ -4430,7 +4436,7 @@
         <v>1088241672</v>
       </c>
       <c r="H35" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I35" s="13">
         <v>44385</v>
@@ -4444,10 +4450,10 @@
         <v>52967870</v>
       </c>
       <c r="C36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E36">
         <v>52967870</v>
@@ -4459,7 +4465,7 @@
         <v>79876965</v>
       </c>
       <c r="H36" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I36" s="13">
         <v>40689</v>
@@ -4473,10 +4479,10 @@
         <v>1088241672</v>
       </c>
       <c r="C37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E37">
         <v>1088241672</v>
@@ -4488,7 +4494,7 @@
         <v>80715371</v>
       </c>
       <c r="H37" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I37" s="13">
         <v>42299</v>
@@ -4502,22 +4508,22 @@
         <v>16283802</v>
       </c>
       <c r="C38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E38">
         <v>16283802</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G38">
         <v>80715371</v>
       </c>
       <c r="H38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I38" s="13">
         <v>43160</v>
@@ -4531,22 +4537,22 @@
         <v>12280914</v>
       </c>
       <c r="C39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E39">
         <v>12280914</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G39">
         <v>16283802</v>
       </c>
       <c r="H39" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I39" s="13">
         <v>44419</v>
@@ -4560,10 +4566,10 @@
         <v>1144192153</v>
       </c>
       <c r="C40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E40">
         <v>1144192153</v>
@@ -4575,7 +4581,7 @@
         <v>80716083</v>
       </c>
       <c r="H40" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I40" s="13">
         <v>44973</v>
@@ -4589,10 +4595,10 @@
         <v>80716083</v>
       </c>
       <c r="C41" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E41">
         <v>80716083</v>
@@ -4604,7 +4610,7 @@
         <v>19437948</v>
       </c>
       <c r="H41" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I41" s="13">
         <v>38940</v>
@@ -4618,10 +4624,10 @@
         <v>1010008125</v>
       </c>
       <c r="C42" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E42">
         <v>1010008125</v>
@@ -4633,7 +4639,7 @@
         <v>80716083</v>
       </c>
       <c r="H42" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I42" s="13">
         <v>45426</v>
@@ -4647,10 +4653,10 @@
         <v>24335303</v>
       </c>
       <c r="C43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E43">
         <v>24335303</v>
@@ -4662,7 +4668,7 @@
         <v>80716083</v>
       </c>
       <c r="H43" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I43" s="13">
         <v>42989</v>
@@ -4676,10 +4682,10 @@
         <v>1100395954</v>
       </c>
       <c r="C44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E44">
         <v>1100395954</v>
@@ -4691,7 +4697,7 @@
         <v>80716083</v>
       </c>
       <c r="H44" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I44" s="13">
         <v>42767</v>
@@ -4705,10 +4711,10 @@
         <v>1020836180</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E45">
         <v>1020836180</v>
@@ -4720,7 +4726,7 @@
         <v>80716083</v>
       </c>
       <c r="H45" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I45" s="13">
         <v>45393</v>
@@ -4734,10 +4740,10 @@
         <v>1130664650</v>
       </c>
       <c r="C46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E46">
         <v>1130664650</v>
@@ -4749,7 +4755,7 @@
         <v>80716083</v>
       </c>
       <c r="H46" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I46" s="13">
         <v>41870</v>
@@ -4763,10 +4769,10 @@
         <v>1026298402</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E47">
         <v>1026298402</v>
@@ -4778,7 +4784,7 @@
         <v>80716083</v>
       </c>
       <c r="H47" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I47" s="13">
         <v>44237</v>
@@ -4792,10 +4798,10 @@
         <v>1073606984</v>
       </c>
       <c r="C48" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E48">
         <v>1073606984</v>
@@ -4807,7 +4813,7 @@
         <v>80716083</v>
       </c>
       <c r="H48" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I48" s="13">
         <v>45414</v>
@@ -4821,10 +4827,10 @@
         <v>1028780316</v>
       </c>
       <c r="C49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E49">
         <v>1028780316</v>
@@ -4836,7 +4842,7 @@
         <v>52374980</v>
       </c>
       <c r="H49" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I49" s="13">
         <v>45406</v>
@@ -4850,22 +4856,22 @@
         <v>1151962737</v>
       </c>
       <c r="C50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E50">
         <v>1151962737</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G50">
         <v>1151937537</v>
       </c>
       <c r="H50" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I50" s="13">
         <v>45019</v>
@@ -4879,22 +4885,22 @@
         <v>94314577</v>
       </c>
       <c r="C51" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E51">
         <v>94314577</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G51">
         <v>1151937537</v>
       </c>
       <c r="H51" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I51" s="13">
         <v>35731</v>
@@ -4908,22 +4914,22 @@
         <v>1144202386</v>
       </c>
       <c r="C52" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E52">
         <v>1144202386</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G52">
         <v>1151937537</v>
       </c>
       <c r="H52" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I52" s="13">
         <v>44690</v>
@@ -4937,22 +4943,22 @@
         <v>1151937537</v>
       </c>
       <c r="C53" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E53">
         <v>1151937537</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G53">
         <v>29545232</v>
       </c>
       <c r="H53" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I53" s="13">
         <v>44256</v>
@@ -4966,10 +4972,10 @@
         <v>1022432298</v>
       </c>
       <c r="C54" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E54">
         <v>1022432298</v>
@@ -4981,7 +4987,7 @@
         <v>52387856</v>
       </c>
       <c r="H54" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I54" s="13">
         <v>45421</v>
@@ -4995,10 +5001,10 @@
         <v>1033679367</v>
       </c>
       <c r="C55" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E55">
         <v>1033679367</v>
@@ -5010,7 +5016,7 @@
         <v>52387856</v>
       </c>
       <c r="H55" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I55" s="13">
         <v>42387</v>
@@ -5024,10 +5030,10 @@
         <v>1032370392</v>
       </c>
       <c r="C56" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E56">
         <v>1032370392</v>
@@ -5039,7 +5045,7 @@
         <v>52387856</v>
       </c>
       <c r="H56" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I56" s="13">
         <v>44546</v>
@@ -5053,10 +5059,10 @@
         <v>31994871</v>
       </c>
       <c r="C57" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E57">
         <v>31994871</v>
@@ -5068,7 +5074,7 @@
         <v>52387856</v>
       </c>
       <c r="H57" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I57" s="13">
         <v>33925</v>
@@ -5082,10 +5088,10 @@
         <v>1032378265</v>
       </c>
       <c r="C58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E58">
         <v>1032378265</v>
@@ -5097,7 +5103,7 @@
         <v>52387856</v>
       </c>
       <c r="H58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I58" s="13">
         <v>45406</v>
@@ -5111,10 +5117,10 @@
         <v>1014266801</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E59">
         <v>1014266801</v>
@@ -5126,7 +5132,7 @@
         <v>52387856</v>
       </c>
       <c r="H59" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I59" s="13">
         <v>42387</v>
@@ -5140,10 +5146,10 @@
         <v>52387856</v>
       </c>
       <c r="C60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E60">
         <v>52387856</v>
@@ -5155,7 +5161,7 @@
         <v>80715371</v>
       </c>
       <c r="H60" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I60" s="13">
         <v>44747</v>
@@ -5169,10 +5175,10 @@
         <v>1112470260</v>
       </c>
       <c r="C61" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E61">
         <v>1112470260</v>
@@ -5184,7 +5190,7 @@
         <v>29545232</v>
       </c>
       <c r="H61" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I61" s="13">
         <v>45069</v>
@@ -5198,10 +5204,10 @@
         <v>1014195964</v>
       </c>
       <c r="C62" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E62">
         <v>1014195964</v>
@@ -5213,7 +5219,7 @@
         <v>11204771</v>
       </c>
       <c r="H62" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I62" s="13">
         <v>45027</v>
@@ -5227,10 +5233,10 @@
         <v>1022372022</v>
       </c>
       <c r="C63" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E63">
         <v>1022372022</v>
@@ -5242,7 +5248,7 @@
         <v>11204771</v>
       </c>
       <c r="H63" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I63" s="13">
         <v>43525</v>
@@ -5256,10 +5262,10 @@
         <v>1144184932</v>
       </c>
       <c r="C64" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E64">
         <v>1144184932</v>
@@ -5271,7 +5277,7 @@
         <v>11204771</v>
       </c>
       <c r="H64" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I64" s="13">
         <v>45097</v>
@@ -5285,10 +5291,10 @@
         <v>52397948</v>
       </c>
       <c r="C65" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E65">
         <v>52397948</v>
@@ -5300,7 +5306,7 @@
         <v>11204771</v>
       </c>
       <c r="H65" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I65" s="13">
         <v>39835</v>
@@ -5314,10 +5320,10 @@
         <v>1082896555</v>
       </c>
       <c r="C66" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E66">
         <v>1082896555</v>
@@ -5329,7 +5335,7 @@
         <v>11204771</v>
       </c>
       <c r="H66" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I66" s="13">
         <v>44546</v>
@@ -5343,10 +5349,10 @@
         <v>11204771</v>
       </c>
       <c r="C67" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E67">
         <v>11204771</v>
@@ -5358,7 +5364,7 @@
         <v>80715371</v>
       </c>
       <c r="H67" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I67" s="13">
         <v>44531</v>
@@ -5372,10 +5378,10 @@
         <v>1022357137</v>
       </c>
       <c r="C68" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E68">
         <v>1022357137</v>
@@ -5387,7 +5393,7 @@
         <v>11204771</v>
       </c>
       <c r="H68" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I68" s="13">
         <v>43873</v>
@@ -5401,22 +5407,22 @@
         <v>43740785</v>
       </c>
       <c r="C69" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E69">
         <v>43740785</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G69">
         <v>80418813</v>
       </c>
       <c r="H69" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I69" s="13">
         <v>44459</v>
@@ -5430,22 +5436,22 @@
         <v>10141808</v>
       </c>
       <c r="C70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E70">
         <v>10141808</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G70">
         <v>80418813</v>
       </c>
       <c r="H70" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I70" s="13">
         <v>39633</v>
@@ -5459,22 +5465,22 @@
         <v>16892353</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E71">
         <v>16892353</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G71">
         <v>1127227679</v>
       </c>
       <c r="H71" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I71" s="13">
         <v>40616</v>
@@ -5488,22 +5494,22 @@
         <v>1014208937</v>
       </c>
       <c r="C72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E72">
         <v>1014208937</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G72">
         <v>80418813</v>
       </c>
       <c r="H72" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I72" s="13">
         <v>42537</v>
@@ -5517,22 +5523,22 @@
         <v>94527898</v>
       </c>
       <c r="C73" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E73">
         <v>94527898</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G73">
         <v>80418813</v>
       </c>
       <c r="H73" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I73" s="13">
         <v>45027</v>
@@ -5546,22 +5552,22 @@
         <v>1061792223</v>
       </c>
       <c r="C74" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E74">
         <v>1061792223</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G74">
         <v>80418813</v>
       </c>
       <c r="H74" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I74" s="13">
         <v>43712</v>
@@ -5575,22 +5581,22 @@
         <v>52799379</v>
       </c>
       <c r="C75" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E75">
         <v>52799379</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G75">
         <v>1127227679</v>
       </c>
       <c r="H75" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I75" s="13">
         <v>43781</v>
@@ -5604,22 +5610,22 @@
         <v>80418813</v>
       </c>
       <c r="C76" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E76">
         <v>80418813</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G76">
         <v>19437948</v>
       </c>
       <c r="H76" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I76" s="13">
         <v>35814</v>
@@ -5633,22 +5639,22 @@
         <v>1014273791</v>
       </c>
       <c r="C77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E77">
         <v>1014273791</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G77">
         <v>80418813</v>
       </c>
       <c r="H77" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I77" s="13">
         <v>44767</v>
@@ -5662,22 +5668,22 @@
         <v>80038307</v>
       </c>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D78" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E78">
         <v>80038307</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G78">
         <v>80418813</v>
       </c>
       <c r="H78" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I78" s="13">
         <v>44718</v>
@@ -5691,22 +5697,22 @@
         <v>1020728518</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D79" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E79">
         <v>1020728518</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G79">
         <v>80418813</v>
       </c>
       <c r="H79" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I79" s="13">
         <v>45056</v>
@@ -5720,22 +5726,22 @@
         <v>1132399033</v>
       </c>
       <c r="C80" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E80">
         <v>1132399033</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G80">
         <v>1127227679</v>
       </c>
       <c r="H80" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I80" s="13">
         <v>43430</v>
@@ -5749,22 +5755,22 @@
         <v>9102465</v>
       </c>
       <c r="C81" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E81">
         <v>9102465</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G81">
         <v>80418813</v>
       </c>
       <c r="H81" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I81" s="13">
         <v>43361</v>
@@ -5778,22 +5784,22 @@
         <v>60352783</v>
       </c>
       <c r="C82" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E82">
         <v>60352783</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G82">
         <v>80418813</v>
       </c>
       <c r="H82" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I82" s="13">
         <v>36419</v>
@@ -5807,22 +5813,22 @@
         <v>79789569</v>
       </c>
       <c r="C83" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E83">
         <v>79789569</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G83">
         <v>80418813</v>
       </c>
       <c r="H83" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I83" s="13">
         <v>45160</v>
@@ -5836,22 +5842,22 @@
         <v>1010030076</v>
       </c>
       <c r="C84" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E84">
         <v>1010030076</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G84">
         <v>80418813</v>
       </c>
       <c r="H84" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I84" s="13">
         <v>45406</v>
@@ -5865,22 +5871,22 @@
         <v>1023902790</v>
       </c>
       <c r="C85" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E85">
         <v>1023902790</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G85">
         <v>1127227679</v>
       </c>
       <c r="H85" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I85" s="13">
         <v>41894</v>
@@ -5894,22 +5900,22 @@
         <v>52443176</v>
       </c>
       <c r="C86" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E86">
         <v>52443176</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G86">
         <v>80418813</v>
       </c>
       <c r="H86" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I86" s="13">
         <v>44781</v>
@@ -5923,22 +5929,22 @@
         <v>16724035</v>
       </c>
       <c r="C87" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E87">
         <v>16724035</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G87">
         <v>94527898</v>
       </c>
       <c r="H87" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I87" s="13">
         <v>36964</v>
@@ -5952,22 +5958,22 @@
         <v>1082842047</v>
       </c>
       <c r="C88" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E88">
         <v>1082842047</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G88">
         <v>80418813</v>
       </c>
       <c r="H88" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I88" s="13">
         <v>41717</v>
@@ -5981,22 +5987,22 @@
         <v>1030587072</v>
       </c>
       <c r="C89" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E89">
         <v>1030587072</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G89">
         <v>80418813</v>
       </c>
       <c r="H89" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I89" s="13">
         <v>43493</v>
@@ -6010,22 +6016,22 @@
         <v>52981547</v>
       </c>
       <c r="C90" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E90">
         <v>52981547</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G90">
         <v>1127227679</v>
       </c>
       <c r="H90" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I90" s="13">
         <v>44789</v>
@@ -6039,22 +6045,22 @@
         <v>29448802</v>
       </c>
       <c r="C91" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E91">
         <v>29448802</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G91">
         <v>94527898</v>
       </c>
       <c r="H91" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I91" s="13">
         <v>36577</v>
@@ -6068,22 +6074,22 @@
         <v>79972267</v>
       </c>
       <c r="C92" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E92">
         <v>79972267</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G92">
         <v>1127227679</v>
       </c>
       <c r="H92" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I92" s="13">
         <v>43605</v>
@@ -6097,22 +6103,22 @@
         <v>9101542</v>
       </c>
       <c r="C93" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E93">
         <v>9101542</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G93">
         <v>1127227679</v>
       </c>
       <c r="H93" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I93" s="13">
         <v>44720</v>
@@ -6126,22 +6132,22 @@
         <v>1140845471</v>
       </c>
       <c r="C94" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E94">
         <v>1140845471</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G94">
         <v>80418813</v>
       </c>
       <c r="H94" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I94" s="13">
         <v>45426</v>
@@ -6155,22 +6161,22 @@
         <v>43258024</v>
       </c>
       <c r="C95" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D95" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E95">
         <v>43258024</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G95">
         <v>80418813</v>
       </c>
       <c r="H95" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I95" s="13">
         <v>43305</v>
@@ -6184,22 +6190,22 @@
         <v>80750426</v>
       </c>
       <c r="C96" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E96">
         <v>80750426</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G96">
         <v>1127227679</v>
       </c>
       <c r="H96" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I96" s="13">
         <v>44986</v>
@@ -6213,22 +6219,22 @@
         <v>66966475</v>
       </c>
       <c r="C97" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E97">
         <v>66966475</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G97">
         <v>39652985</v>
       </c>
       <c r="H97" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I97" s="13">
         <v>37895</v>
@@ -6242,22 +6248,22 @@
         <v>1000805726</v>
       </c>
       <c r="C98" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E98">
         <v>1000805726</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G98">
         <v>1127227679</v>
       </c>
       <c r="H98" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I98" s="13">
         <v>45152</v>
@@ -6271,22 +6277,22 @@
         <v>1032452403</v>
       </c>
       <c r="C99" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E99">
         <v>1032452403</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G99">
         <v>80418813</v>
       </c>
       <c r="H99" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I99" s="13">
         <v>45426</v>
@@ -6300,22 +6306,22 @@
         <v>39652985</v>
       </c>
       <c r="C100" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E100">
         <v>39652985</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G100">
         <v>80418813</v>
       </c>
       <c r="H100" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I100" s="13">
         <v>36035</v>
@@ -6329,22 +6335,22 @@
         <v>19437948</v>
       </c>
       <c r="C101" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E101">
         <v>19437948</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G101">
         <v>19437948</v>
       </c>
       <c r="H101" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I101" s="13">
         <v>42675</v>
@@ -6358,22 +6364,22 @@
         <v>1127227679</v>
       </c>
       <c r="C102" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E102">
         <v>1127227679</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G102">
         <v>19437948</v>
       </c>
       <c r="H102" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I102" s="13">
         <v>40371</v>
@@ -6387,22 +6393,22 @@
         <v>52825105</v>
       </c>
       <c r="C103" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E103">
         <v>52825105</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G103">
         <v>80418813</v>
       </c>
       <c r="H103" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I103" s="13">
         <v>41891</v>
@@ -6416,22 +6422,22 @@
         <v>1037620057</v>
       </c>
       <c r="C104" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E104">
         <v>1037620057</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G104">
         <v>1127227679</v>
       </c>
       <c r="H104" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I104" s="13">
         <v>45090</v>
@@ -6445,22 +6451,22 @@
         <v>53092348</v>
       </c>
       <c r="C105" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E105">
         <v>53092348</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G105">
         <v>80418813</v>
       </c>
       <c r="H105" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I105" s="13">
         <v>45001</v>
@@ -6474,22 +6480,22 @@
         <v>52829740</v>
       </c>
       <c r="C106" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E106">
         <v>52829740</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G106">
         <v>80418813</v>
       </c>
       <c r="H106" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I106" s="13">
         <v>44692</v>
@@ -6503,22 +6509,22 @@
         <v>80197944</v>
       </c>
       <c r="C107" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E107">
         <v>80197944</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G107">
         <v>19437948</v>
       </c>
       <c r="H107" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I107" s="13">
         <v>45049</v>
@@ -6532,22 +6538,22 @@
         <v>52875283</v>
       </c>
       <c r="C108" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E108">
         <v>52875283</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G108">
         <v>80418813</v>
       </c>
       <c r="H108" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I108" s="13">
         <v>42866</v>
@@ -6561,22 +6567,22 @@
         <v>98348118</v>
       </c>
       <c r="C109" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E109">
         <v>98348118</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G109">
         <v>1127227679</v>
       </c>
       <c r="H109" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I109" s="13">
         <v>42304</v>
@@ -6590,22 +6596,22 @@
         <v>53069619</v>
       </c>
       <c r="C110" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E110">
         <v>53069619</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G110">
         <v>1127227679</v>
       </c>
       <c r="H110" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I110" s="13">
         <v>41864</v>
@@ -6619,10 +6625,10 @@
         <v>4563456</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E111" s="20">
         <v>4563456</v>
@@ -6632,7 +6638,7 @@
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I111" s="13">
         <v>45437</v>
@@ -6646,10 +6652,10 @@
         <v>3456435</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D112" s="19" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E112" s="20">
         <v>3456435</v>
@@ -6659,7 +6665,7 @@
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I112" s="13">
         <v>45437</v>
@@ -6734,10 +6740,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D3" t="s">
         <v>64</v>
@@ -6785,10 +6791,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -6802,16 +6808,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" t="s">
         <v>157</v>
-      </c>
-      <c r="C7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -6862,7 +6868,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -6913,7 +6919,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -6946,7 +6952,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -6957,10 +6963,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -7025,7 +7031,7 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E2" t="s">
         <v>89</v>
@@ -7045,13 +7051,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E3" t="s">
         <v>90</v>
@@ -7071,13 +7077,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E4" t="s">
         <v>91</v>
@@ -7103,7 +7109,7 @@
         <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E5" t="s">
         <v>92</v>
@@ -7112,10 +7118,10 @@
         <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -7129,7 +7135,7 @@
         <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E6" t="s">
         <v>93</v>
@@ -7138,10 +7144,10 @@
         <v>93</v>
       </c>
       <c r="G6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7149,19 +7155,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G7" t="s">
         <v>68</v>
@@ -7175,19 +7181,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D8" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G8" t="s">
         <v>69</v>
@@ -7201,13 +7207,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D9" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E9" t="s">
         <v>94</v>
@@ -7233,7 +7239,7 @@
         <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E10" t="s">
         <v>95</v>
@@ -7259,7 +7265,7 @@
         <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E11" t="s">
         <v>96</v>
@@ -7279,19 +7285,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G12" t="s">
         <v>72</v>
@@ -7305,19 +7311,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G13" t="s">
         <v>72</v>
@@ -7331,10 +7337,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D14" t="s">
         <v>60</v>
@@ -7357,10 +7363,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D15" t="s">
         <v>60</v>
@@ -7383,10 +7389,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D16" t="s">
         <v>60</v>
@@ -7409,10 +7415,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D17" t="s">
         <v>60</v>
@@ -7435,10 +7441,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D18" t="s">
         <v>60</v>
@@ -7450,10 +7456,10 @@
         <v>84</v>
       </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -7461,10 +7467,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D19" t="s">
         <v>60</v>
@@ -7476,10 +7482,10 @@
         <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -7487,10 +7493,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C20" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
@@ -7513,10 +7519,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C21" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D21" t="s">
         <v>60</v>
@@ -7539,10 +7545,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C22" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D22" t="s">
         <v>60</v>
@@ -7554,10 +7560,10 @@
         <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -7565,10 +7571,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D23" t="s">
         <v>60</v>
@@ -7591,10 +7597,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
@@ -7606,10 +7612,10 @@
         <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -7617,10 +7623,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C25" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D25" t="s">
         <v>60</v>
@@ -7632,10 +7638,10 @@
         <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -7643,25 +7649,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C26" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D26" t="s">
         <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F26" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -7669,13 +7675,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>481</v>
+      </c>
+      <c r="C27" t="s">
+        <v>481</v>
+      </c>
+      <c r="D27" t="s">
         <v>483</v>
-      </c>
-      <c r="C27" t="s">
-        <v>483</v>
-      </c>
-      <c r="D27" t="s">
-        <v>485</v>
       </c>
       <c r="E27" t="s">
         <v>97</v>
@@ -7684,10 +7690,10 @@
         <v>97</v>
       </c>
       <c r="G27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -7695,25 +7701,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D28" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -7721,25 +7727,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D29" t="s">
         <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -7747,25 +7753,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -7773,13 +7779,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C31" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D31" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E31" t="s">
         <v>100</v>
@@ -7805,13 +7811,13 @@
         <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G32" t="s">
         <v>65</v>
@@ -7831,13 +7837,13 @@
         <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G33" t="s">
         <v>66</v>
@@ -7857,13 +7863,13 @@
         <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G34" t="s">
         <v>66</v>
@@ -7883,13 +7889,13 @@
         <v>126</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G35" t="s">
         <v>66</v>
@@ -7909,13 +7915,13 @@
         <v>127</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" t="s">
         <v>66</v>
@@ -7935,19 +7941,19 @@
         <v>128</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -7961,19 +7967,19 @@
         <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -7987,19 +7993,19 @@
         <v>130</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -8013,13 +8019,13 @@
         <v>131</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G40" t="s">
         <v>68</v>
@@ -8039,13 +8045,13 @@
         <v>132</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G41" t="s">
         <v>69</v>
@@ -8065,13 +8071,13 @@
         <v>133</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G42" t="s">
         <v>70</v>
@@ -8085,19 +8091,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C43" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G43" t="s">
         <v>72</v>
@@ -8117,13 +8123,13 @@
         <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G44" t="s">
         <v>71</v>
@@ -8137,19 +8143,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C45" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G45" t="s">
         <v>67</v>
@@ -8314,7 +8320,7 @@
         <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8347,7 +8353,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8355,10 +8361,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" t="s">
         <v>158</v>
-      </c>
-      <c r="C9" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar ingrid.valero@finac.com para tests
</commit_message>
<xml_diff>
--- a/backend/data/IRA_data.xlsx
+++ b/backend/data/IRA_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA50629-8E96-5A46-98B1-F4EFA1B5CFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D812271-29C5-3149-8AD7-9F8DC187C2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22100" yWindow="11020" windowWidth="39120" windowHeight="23400" activeTab="12" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
+    <workbookView xWindow="12080" yWindow="4340" windowWidth="39120" windowHeight="23400" activeTab="2" xr2:uid="{52CC5870-0867-48B7-840C-744248B71BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Periodo" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="514">
   <si>
     <t>Nombre_es</t>
   </si>
@@ -1577,6 +1577,12 @@
   </si>
   <si>
     <t>NARRATIVA 2: Una situación que Usted ha observado, que haya tenido dificultades y que esas dificultades hubieran sido menores si hubiera existido mejor comunicación y coordinación de tareas entre áreas. Trate de explicar cuáles fueron las dificultades en comunicación y coordinación, y en lo posible sugiera cómo estas cosas hubieran podido ser mejores. Indique, a su modo de ver, si esto tuvo impacto sobre el cliente y por qué o por qué no. Sea lo más específico posible.</t>
+  </si>
+  <si>
+    <t>Ingrid Valero</t>
+  </si>
+  <si>
+    <t>ingrid.valero@finac.com</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1712,6 +1718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3160,7 +3167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3042CE92-63A8-44A4-B4EF-831678C97DF5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3408,10 +3415,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C248DF4-33E4-45F0-A9B3-DCFFCEC7ACF1}">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6663,12 +6670,43 @@
       <c r="F112" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G112" s="4"/>
+      <c r="G112" s="20">
+        <v>4563456</v>
+      </c>
       <c r="H112" s="4" t="s">
         <v>509</v>
       </c>
       <c r="I112" s="13">
         <v>45437</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>678978</v>
+      </c>
+      <c r="C113" t="s">
+        <v>512</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>513</v>
+      </c>
+      <c r="E113">
+        <v>678978</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G113" s="20">
+        <v>4563456</v>
+      </c>
+      <c r="H113" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="I113" s="13">
+        <v>45438</v>
       </c>
     </row>
   </sheetData>
@@ -6678,9 +6716,10 @@
     <hyperlink ref="D4" r:id="rId3" display="ingrid.valero@finac.com" xr:uid="{D942AD9A-8C2A-2048-AEEA-ED0633100CD3}"/>
     <hyperlink ref="D111" r:id="rId4" xr:uid="{2BA97543-D197-D645-BF59-02D4CE2B8321}"/>
     <hyperlink ref="D112" r:id="rId5" xr:uid="{F4386B81-EAAC-5744-B967-60779B565C3B}"/>
+    <hyperlink ref="D113" r:id="rId6" xr:uid="{1A93D8DD-B5DC-A543-B882-5D9D96B6205E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>